<commit_message>
test: add analysis result
</commit_message>
<xml_diff>
--- a/FP_result.xlsx
+++ b/FP_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy\Desktop\code_ress\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BDED57-708A-4F32-B454-9D11541BDAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF2C915-C100-4103-86DE-43912CECC798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="63">
   <si>
     <t>FP</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -257,7 +257,29 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>检测成本，defect时间越靠后，失效概率越大</t>
+    <t>检测成本，defect时间越靠后，MI无效开销越多</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sensitivity analysis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model B</t>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proposed policy</t>
+  </si>
+  <si>
+    <t>Savings</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -269,7 +291,7 @@
     <numFmt numFmtId="176" formatCode="#,##0.000"/>
     <numFmt numFmtId="177" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +328,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,8 +382,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -506,6 +562,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -513,7 +578,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -569,10 +634,70 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1271,25 +1396,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DEFD31-C20C-4FCF-BDFB-E8B3E171E50B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="4.9140625" customWidth="1"/>
+    <col min="12" max="12" width="1.25" customWidth="1"/>
+    <col min="16" max="16" width="1.25" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="32"/>
+      <c r="J1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="11" t="s">
         <v>36</v>
@@ -1304,7 +1439,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>44</v>
       </c>
@@ -1318,8 +1453,27 @@
         <v>34</v>
       </c>
       <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J3" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>20</v>
       </c>
@@ -1335,8 +1489,35 @@
       <c r="E4" s="12">
         <v>6.4233000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="T4" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
@@ -1352,8 +1533,47 @@
       <c r="E5" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="36">
+        <f>'sensi_speed cs'!A2</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36">
+        <f>'sensi_speed cs'!C2</f>
+        <v>21</v>
+      </c>
+      <c r="N5" s="36">
+        <f>'sensi_speed cs'!D2</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="36">
+        <f>'sensi_speed cs'!E2</f>
+        <v>5.8662999999999998</v>
+      </c>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36">
+        <f>'sensi_speed cs'!F2</f>
+        <v>9</v>
+      </c>
+      <c r="R5" s="36">
+        <f>'sensi_speed cs'!G2</f>
+        <v>12</v>
+      </c>
+      <c r="S5" s="36">
+        <f>'sensi_speed cs'!H2</f>
+        <v>7.9919000000000002</v>
+      </c>
+      <c r="T5" s="37">
+        <f>'sensi_speed cs'!I2</f>
+        <v>0.265969293910084</v>
+      </c>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -1373,11 +1593,1665 @@
         <f>(E4-$E$4)/E4</f>
         <v>0</v>
       </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="44">
+        <f>'sensi_speed cs'!A3</f>
+        <v>5</v>
+      </c>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44">
+        <f>'sensi_speed cs'!C3</f>
+        <v>18</v>
+      </c>
+      <c r="N6" s="44">
+        <f>'sensi_speed cs'!D3</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O6" s="44">
+        <f>'sensi_speed cs'!E3</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44">
+        <f>'sensi_speed cs'!F3</f>
+        <v>9</v>
+      </c>
+      <c r="R6" s="44">
+        <f>'sensi_speed cs'!G3</f>
+        <v>12</v>
+      </c>
+      <c r="S6" s="44">
+        <f>'sensi_speed cs'!H3</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T6" s="45">
+        <f>'sensi_speed cs'!I3</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J7" s="35"/>
+      <c r="K7" s="36">
+        <f>'sensi_speed cs'!A4</f>
+        <v>8</v>
+      </c>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36">
+        <f>'sensi_speed cs'!C4</f>
+        <v>19</v>
+      </c>
+      <c r="N7" s="36">
+        <f>'sensi_speed cs'!D4</f>
+        <v>1.2</v>
+      </c>
+      <c r="O7" s="36">
+        <f>'sensi_speed cs'!E4</f>
+        <v>6.8905000000000003</v>
+      </c>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36">
+        <f>'sensi_speed cs'!F4</f>
+        <v>9</v>
+      </c>
+      <c r="R7" s="36">
+        <f>'sensi_speed cs'!G4</f>
+        <v>12</v>
+      </c>
+      <c r="S7" s="36">
+        <f>'sensi_speed cs'!H4</f>
+        <v>8.6296999999999997</v>
+      </c>
+      <c r="T7" s="37">
+        <f>'sensi_speed cs'!I4</f>
+        <v>0.20153655399376566</v>
+      </c>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J8" s="35"/>
+      <c r="K8" s="36">
+        <f>'sensi_speed cs'!A5</f>
+        <v>11</v>
+      </c>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36">
+        <f>'sensi_speed cs'!C5</f>
+        <v>16</v>
+      </c>
+      <c r="N8" s="36">
+        <f>'sensi_speed cs'!D5</f>
+        <v>1</v>
+      </c>
+      <c r="O8" s="36">
+        <f>'sensi_speed cs'!E5</f>
+        <v>7.3307000000000002</v>
+      </c>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36">
+        <f>'sensi_speed cs'!F5</f>
+        <v>9</v>
+      </c>
+      <c r="R8" s="36">
+        <f>'sensi_speed cs'!G5</f>
+        <v>12</v>
+      </c>
+      <c r="S8" s="36">
+        <f>'sensi_speed cs'!H5</f>
+        <v>8.9352</v>
+      </c>
+      <c r="T8" s="37">
+        <f>'sensi_speed cs'!I5</f>
+        <v>0.17957068672217744</v>
+      </c>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J9" s="38"/>
+      <c r="K9" s="34">
+        <f>'sensi_speed cs'!A6</f>
+        <v>14</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34">
+        <f>'sensi_speed cs'!C6</f>
+        <v>16</v>
+      </c>
+      <c r="N9" s="34">
+        <f>'sensi_speed cs'!D6</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="34">
+        <f>'sensi_speed cs'!E6</f>
+        <v>7.7404000000000002</v>
+      </c>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34">
+        <f>'sensi_speed cs'!F6</f>
+        <v>9</v>
+      </c>
+      <c r="R9" s="34">
+        <f>'sensi_speed cs'!G6</f>
+        <v>12</v>
+      </c>
+      <c r="S9" s="34">
+        <f>'sensi_speed cs'!H6</f>
+        <v>9.3028999999999993</v>
+      </c>
+      <c r="T9" s="39">
+        <f>'sensi_speed cs'!I6</f>
+        <v>0.16795837857012322</v>
+      </c>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J10" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="41">
+        <f>'sensi_speed cs'!A12</f>
+        <v>10</v>
+      </c>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41">
+        <f>'sensi_speed cs'!C12</f>
+        <v>18</v>
+      </c>
+      <c r="N10" s="41">
+        <f>'sensi_speed cs'!D12</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="41">
+        <f>'sensi_speed cs'!E12</f>
+        <v>6.4054000000000002</v>
+      </c>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41">
+        <f>'sensi_speed cs'!F12</f>
+        <v>9</v>
+      </c>
+      <c r="R10" s="41">
+        <f>'sensi_speed cs'!G12</f>
+        <v>12</v>
+      </c>
+      <c r="S10" s="41">
+        <f>'sensi_speed cs'!H12</f>
+        <v>8.0942000000000007</v>
+      </c>
+      <c r="T10" s="42">
+        <f>'sensi_speed cs'!I12</f>
+        <v>0.20864322601368887</v>
+      </c>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7">
+        <f>'sensi_speed cs'!K12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J11" s="35"/>
+      <c r="K11" s="44">
+        <f>'sensi_speed cs'!A13</f>
+        <v>15</v>
+      </c>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44">
+        <f>'sensi_speed cs'!C13</f>
+        <v>18</v>
+      </c>
+      <c r="N11" s="44">
+        <f>'sensi_speed cs'!D13</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O11" s="44">
+        <f>'sensi_speed cs'!E13</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44">
+        <f>'sensi_speed cs'!F13</f>
+        <v>9</v>
+      </c>
+      <c r="R11" s="44">
+        <f>'sensi_speed cs'!G13</f>
+        <v>12</v>
+      </c>
+      <c r="S11" s="44">
+        <f>'sensi_speed cs'!H13</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T11" s="45">
+        <f>'sensi_speed cs'!I13</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7">
+        <f>'sensi_speed cs'!K13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J12" s="35"/>
+      <c r="K12" s="36">
+        <f>'sensi_speed cs'!A14</f>
+        <v>20</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36">
+        <f>'sensi_speed cs'!C14</f>
+        <v>18</v>
+      </c>
+      <c r="N12" s="36">
+        <f>'sensi_speed cs'!D14</f>
+        <v>1.3</v>
+      </c>
+      <c r="O12" s="36">
+        <f>'sensi_speed cs'!E14</f>
+        <v>6.4127000000000001</v>
+      </c>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36">
+        <f>'sensi_speed cs'!F14</f>
+        <v>9</v>
+      </c>
+      <c r="R12" s="36">
+        <f>'sensi_speed cs'!G14</f>
+        <v>12</v>
+      </c>
+      <c r="S12" s="36">
+        <f>'sensi_speed cs'!H14</f>
+        <v>8.5197000000000003</v>
+      </c>
+      <c r="T12" s="37">
+        <f>'sensi_speed cs'!I14</f>
+        <v>0.24730917755320025</v>
+      </c>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7">
+        <f>'sensi_speed cs'!K14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J13" s="35"/>
+      <c r="K13" s="36">
+        <f>'sensi_speed cs'!A15</f>
+        <v>25</v>
+      </c>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36">
+        <f>'sensi_speed cs'!C15</f>
+        <v>18</v>
+      </c>
+      <c r="N13" s="36">
+        <f>'sensi_speed cs'!D15</f>
+        <v>0.9</v>
+      </c>
+      <c r="O13" s="36">
+        <f>'sensi_speed cs'!E15</f>
+        <v>6.4028999999999998</v>
+      </c>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36">
+        <f>'sensi_speed cs'!F15</f>
+        <v>9</v>
+      </c>
+      <c r="R13" s="36">
+        <f>'sensi_speed cs'!G15</f>
+        <v>12</v>
+      </c>
+      <c r="S13" s="36">
+        <f>'sensi_speed cs'!H15</f>
+        <v>8.8023000000000007</v>
+      </c>
+      <c r="T13" s="37">
+        <f>'sensi_speed cs'!I15</f>
+        <v>0.27258784635833821</v>
+      </c>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7">
+        <f>'sensi_speed cs'!K15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J14" s="38"/>
+      <c r="K14" s="34">
+        <f>'sensi_speed cs'!A16</f>
+        <v>30</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34">
+        <f>'sensi_speed cs'!C16</f>
+        <v>18</v>
+      </c>
+      <c r="N14" s="34">
+        <f>'sensi_speed cs'!D16</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="34">
+        <f>'sensi_speed cs'!E16</f>
+        <v>6.4105999999999996</v>
+      </c>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34">
+        <f>'sensi_speed cs'!F16</f>
+        <v>9</v>
+      </c>
+      <c r="R14" s="34">
+        <f>'sensi_speed cs'!G16</f>
+        <v>12</v>
+      </c>
+      <c r="S14" s="34">
+        <f>'sensi_speed cs'!H16</f>
+        <v>9.0268999999999995</v>
+      </c>
+      <c r="T14" s="39">
+        <f>'sensi_speed cs'!I16</f>
+        <v>0.28983371921700696</v>
+      </c>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7">
+        <f>'sensi_speed cs'!K16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J15" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="41">
+        <f>'sensi_speed cs'!A23</f>
+        <v>100</v>
+      </c>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41">
+        <f>'sensi_speed cs'!C23</f>
+        <v>18</v>
+      </c>
+      <c r="N15" s="41">
+        <f>'sensi_speed cs'!D23</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O15" s="41">
+        <f>'sensi_speed cs'!E23</f>
+        <v>3.6124999999999998</v>
+      </c>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41">
+        <f>'sensi_speed cs'!F23</f>
+        <v>9</v>
+      </c>
+      <c r="R15" s="41">
+        <f>'sensi_speed cs'!G23</f>
+        <v>11</v>
+      </c>
+      <c r="S15" s="41">
+        <f>'sensi_speed cs'!H23</f>
+        <v>5.0346000000000002</v>
+      </c>
+      <c r="T15" s="42">
+        <f>'sensi_speed cs'!I23</f>
+        <v>0.28246533984825017</v>
+      </c>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7">
+        <f>'sensi_speed cs'!K23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J16" s="38"/>
+      <c r="K16" s="36">
+        <f>'sensi_speed cs'!A24</f>
+        <v>150</v>
+      </c>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36">
+        <f>'sensi_speed cs'!C24</f>
+        <v>18</v>
+      </c>
+      <c r="N16" s="36">
+        <f>'sensi_speed cs'!D24</f>
+        <v>0.8</v>
+      </c>
+      <c r="O16" s="36">
+        <f>'sensi_speed cs'!E24</f>
+        <v>5.0114000000000001</v>
+      </c>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36">
+        <f>'sensi_speed cs'!F24</f>
+        <v>10</v>
+      </c>
+      <c r="R16" s="36">
+        <f>'sensi_speed cs'!G24</f>
+        <v>9</v>
+      </c>
+      <c r="S16" s="36">
+        <f>'sensi_speed cs'!H24</f>
+        <v>6.7560000000000002</v>
+      </c>
+      <c r="T16" s="37">
+        <f>'sensi_speed cs'!I24</f>
+        <v>0.25822972172883363</v>
+      </c>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7">
+        <f>'sensi_speed cs'!K24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J17" s="38"/>
+      <c r="K17" s="44">
+        <f>'sensi_speed cs'!A25</f>
+        <v>200</v>
+      </c>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44">
+        <f>'sensi_speed cs'!C25</f>
+        <v>18</v>
+      </c>
+      <c r="N17" s="44">
+        <f>'sensi_speed cs'!D25</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O17" s="44">
+        <f>'sensi_speed cs'!E25</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44">
+        <f>'sensi_speed cs'!F25</f>
+        <v>9</v>
+      </c>
+      <c r="R17" s="44">
+        <f>'sensi_speed cs'!G25</f>
+        <v>12</v>
+      </c>
+      <c r="S17" s="44">
+        <f>'sensi_speed cs'!H25</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T17" s="45">
+        <f>'sensi_speed cs'!I25</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7">
+        <f>'sensi_speed cs'!K25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J18" s="38"/>
+      <c r="K18" s="36">
+        <f>'sensi_speed cs'!A26</f>
+        <v>250</v>
+      </c>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36">
+        <f>'sensi_speed cs'!C26</f>
+        <v>18</v>
+      </c>
+      <c r="N18" s="36">
+        <f>'sensi_speed cs'!D26</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O18" s="36">
+        <f>'sensi_speed cs'!E26</f>
+        <v>7.8053999999999997</v>
+      </c>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36">
+        <f>'sensi_speed cs'!F26</f>
+        <v>9</v>
+      </c>
+      <c r="R18" s="36">
+        <f>'sensi_speed cs'!G26</f>
+        <v>12</v>
+      </c>
+      <c r="S18" s="36">
+        <f>'sensi_speed cs'!H26</f>
+        <v>10.026400000000001</v>
+      </c>
+      <c r="T18" s="37">
+        <f>'sensi_speed cs'!I26</f>
+        <v>0.22151519987233712</v>
+      </c>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7">
+        <f>'sensi_speed cs'!K26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J19" s="38"/>
+      <c r="K19" s="34">
+        <f>'sensi_speed cs'!A27</f>
+        <v>300</v>
+      </c>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34">
+        <f>'sensi_speed cs'!C27</f>
+        <v>19</v>
+      </c>
+      <c r="N19" s="34">
+        <f>'sensi_speed cs'!D27</f>
+        <v>1.4</v>
+      </c>
+      <c r="O19" s="34">
+        <f>'sensi_speed cs'!E27</f>
+        <v>9.1647999999999996</v>
+      </c>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34">
+        <f>'sensi_speed cs'!F27</f>
+        <v>9</v>
+      </c>
+      <c r="R19" s="34">
+        <f>'sensi_speed cs'!G27</f>
+        <v>13</v>
+      </c>
+      <c r="S19" s="34">
+        <f>'sensi_speed cs'!H27</f>
+        <v>11.72</v>
+      </c>
+      <c r="T19" s="39">
+        <f>'sensi_speed cs'!I27</f>
+        <v>0.21802047781569975</v>
+      </c>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7">
+        <f>'sensi_speed cs'!K27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J20" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="41">
+        <f>'sensi_speed cs'!A34</f>
+        <v>1500</v>
+      </c>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41">
+        <f>'sensi_speed cs'!C34</f>
+        <v>18</v>
+      </c>
+      <c r="N20" s="41">
+        <f>'sensi_speed cs'!D34</f>
+        <v>0.9</v>
+      </c>
+      <c r="O20" s="41">
+        <f>'sensi_speed cs'!E34</f>
+        <v>6.4108999999999998</v>
+      </c>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41">
+        <f>'sensi_speed cs'!F34</f>
+        <v>9</v>
+      </c>
+      <c r="R20" s="41">
+        <f>'sensi_speed cs'!G34</f>
+        <v>13</v>
+      </c>
+      <c r="S20" s="41">
+        <f>'sensi_speed cs'!H34</f>
+        <v>8.2538</v>
+      </c>
+      <c r="T20" s="42">
+        <f>'sensi_speed cs'!I34</f>
+        <v>0.22327897453294243</v>
+      </c>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7">
+        <f>'sensi_speed cs'!K34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J21" s="35"/>
+      <c r="K21" s="44">
+        <f>'sensi_speed cs'!A35</f>
+        <v>2000</v>
+      </c>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44">
+        <f>'sensi_speed cs'!C35</f>
+        <v>18</v>
+      </c>
+      <c r="N21" s="44">
+        <f>'sensi_speed cs'!D35</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O21" s="44">
+        <f>'sensi_speed cs'!E35</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44">
+        <f>'sensi_speed cs'!F35</f>
+        <v>9</v>
+      </c>
+      <c r="R21" s="44">
+        <f>'sensi_speed cs'!G35</f>
+        <v>12</v>
+      </c>
+      <c r="S21" s="44">
+        <f>'sensi_speed cs'!H35</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T21" s="45">
+        <f>'sensi_speed cs'!I35</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7">
+        <f>'sensi_speed cs'!K35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J22" s="35"/>
+      <c r="K22" s="36">
+        <f>'sensi_speed cs'!A36</f>
+        <v>2500</v>
+      </c>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36">
+        <f>'sensi_speed cs'!C36</f>
+        <v>18</v>
+      </c>
+      <c r="N22" s="36">
+        <f>'sensi_speed cs'!D36</f>
+        <v>0.9</v>
+      </c>
+      <c r="O22" s="36">
+        <f>'sensi_speed cs'!E36</f>
+        <v>6.4051999999999998</v>
+      </c>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36">
+        <f>'sensi_speed cs'!F36</f>
+        <v>9</v>
+      </c>
+      <c r="R22" s="36">
+        <f>'sensi_speed cs'!G36</f>
+        <v>12</v>
+      </c>
+      <c r="S22" s="36">
+        <f>'sensi_speed cs'!H36</f>
+        <v>8.3809000000000005</v>
+      </c>
+      <c r="T22" s="37">
+        <f>'sensi_speed cs'!I36</f>
+        <v>0.23573840518321429</v>
+      </c>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7">
+        <f>'sensi_speed cs'!K36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J23" s="35"/>
+      <c r="K23" s="36">
+        <f>'sensi_speed cs'!A37</f>
+        <v>3000</v>
+      </c>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36">
+        <f>'sensi_speed cs'!C37</f>
+        <v>18</v>
+      </c>
+      <c r="N23" s="36">
+        <f>'sensi_speed cs'!D37</f>
+        <v>1.4</v>
+      </c>
+      <c r="O23" s="36">
+        <f>'sensi_speed cs'!E37</f>
+        <v>6.4229000000000003</v>
+      </c>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36">
+        <f>'sensi_speed cs'!F37</f>
+        <v>9</v>
+      </c>
+      <c r="R23" s="36">
+        <f>'sensi_speed cs'!G37</f>
+        <v>12</v>
+      </c>
+      <c r="S23" s="36">
+        <f>'sensi_speed cs'!H37</f>
+        <v>8.4442000000000004</v>
+      </c>
+      <c r="T23" s="37">
+        <f>'sensi_speed cs'!I37</f>
+        <v>0.23937140285639846</v>
+      </c>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7">
+        <f>'sensi_speed cs'!K37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J24" s="38"/>
+      <c r="K24" s="34">
+        <f>'sensi_speed cs'!A38</f>
+        <v>3500</v>
+      </c>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34">
+        <f>'sensi_speed cs'!C38</f>
+        <v>18</v>
+      </c>
+      <c r="N24" s="34">
+        <f>'sensi_speed cs'!D38</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O24" s="34">
+        <f>'sensi_speed cs'!E38</f>
+        <v>6.4227999999999996</v>
+      </c>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34">
+        <f>'sensi_speed cs'!F38</f>
+        <v>9</v>
+      </c>
+      <c r="R24" s="34">
+        <f>'sensi_speed cs'!G38</f>
+        <v>11</v>
+      </c>
+      <c r="S24" s="34">
+        <f>'sensi_speed cs'!H38</f>
+        <v>8.4097000000000008</v>
+      </c>
+      <c r="T24" s="39">
+        <f>'sensi_speed cs'!I38</f>
+        <v>0.23626288690440814</v>
+      </c>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7">
+        <f>'sensi_speed cs'!K38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J25" s="40" t="str">
+        <f>'sensi_speed cs'!A42</f>
+        <v>cs</v>
+      </c>
+      <c r="K25" s="41">
+        <f>'sensi_speed cs'!A43</f>
+        <v>20</v>
+      </c>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41">
+        <f>'sensi_speed cs'!C43</f>
+        <v>18</v>
+      </c>
+      <c r="N25" s="41">
+        <f>'sensi_speed cs'!D43</f>
+        <v>0.9</v>
+      </c>
+      <c r="O25" s="41">
+        <f>'sensi_speed cs'!E43</f>
+        <v>6.4108999999999998</v>
+      </c>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41">
+        <f>'sensi_speed cs'!F43</f>
+        <v>9</v>
+      </c>
+      <c r="R25" s="41">
+        <f>'sensi_speed cs'!G43</f>
+        <v>13</v>
+      </c>
+      <c r="S25" s="41">
+        <f>'sensi_speed cs'!H43</f>
+        <v>8.3396000000000008</v>
+      </c>
+      <c r="T25" s="42">
+        <f>'sensi_speed cs'!I43</f>
+        <v>0.23127008489615819</v>
+      </c>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7">
+        <f>'sensi_speed cs'!K43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J26" s="35"/>
+      <c r="K26" s="36">
+        <f>'sensi_speed cs'!A44</f>
+        <v>30</v>
+      </c>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36">
+        <f>'sensi_speed cs'!C44</f>
+        <v>18</v>
+      </c>
+      <c r="N26" s="36">
+        <f>'sensi_speed cs'!D44</f>
+        <v>1</v>
+      </c>
+      <c r="O26" s="36">
+        <f>'sensi_speed cs'!E44</f>
+        <v>6.4054000000000002</v>
+      </c>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36">
+        <f>'sensi_speed cs'!F44</f>
+        <v>9</v>
+      </c>
+      <c r="R26" s="36">
+        <f>'sensi_speed cs'!G44</f>
+        <v>12</v>
+      </c>
+      <c r="S26" s="36">
+        <f>'sensi_speed cs'!H44</f>
+        <v>8.3114000000000008</v>
+      </c>
+      <c r="T26" s="37">
+        <f>'sensi_speed cs'!I44</f>
+        <v>0.22932357966166955</v>
+      </c>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7">
+        <f>'sensi_speed cs'!K44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J27" s="35"/>
+      <c r="K27" s="44">
+        <f>'sensi_speed cs'!A45</f>
+        <v>40</v>
+      </c>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44">
+        <f>'sensi_speed cs'!C45</f>
+        <v>18</v>
+      </c>
+      <c r="N27" s="44">
+        <f>'sensi_speed cs'!D45</f>
+        <v>1</v>
+      </c>
+      <c r="O27" s="44">
+        <f>'sensi_speed cs'!E45</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44">
+        <f>'sensi_speed cs'!F45</f>
+        <v>9</v>
+      </c>
+      <c r="R27" s="44">
+        <f>'sensi_speed cs'!G45</f>
+        <v>12</v>
+      </c>
+      <c r="S27" s="44">
+        <f>'sensi_speed cs'!H45</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T27" s="45">
+        <f>'sensi_speed cs'!I45</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7">
+        <f>'sensi_speed cs'!K45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J28" s="35"/>
+      <c r="K28" s="36">
+        <f>'sensi_speed cs'!A46</f>
+        <v>50</v>
+      </c>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36">
+        <f>'sensi_speed cs'!C46</f>
+        <v>18</v>
+      </c>
+      <c r="N28" s="36">
+        <f>'sensi_speed cs'!D46</f>
+        <v>1.4</v>
+      </c>
+      <c r="O28" s="36">
+        <f>'sensi_speed cs'!E46</f>
+        <v>6.4229000000000003</v>
+      </c>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36">
+        <f>'sensi_speed cs'!F46</f>
+        <v>9</v>
+      </c>
+      <c r="R28" s="36">
+        <f>'sensi_speed cs'!G46</f>
+        <v>12</v>
+      </c>
+      <c r="S28" s="36">
+        <f>'sensi_speed cs'!H46</f>
+        <v>8.3124000000000002</v>
+      </c>
+      <c r="T28" s="37">
+        <f>'sensi_speed cs'!I46</f>
+        <v>0.22731100524517586</v>
+      </c>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7">
+        <f>'sensi_speed cs'!K46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J29" s="38"/>
+      <c r="K29" s="34">
+        <f>'sensi_speed cs'!A47</f>
+        <v>60</v>
+      </c>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34">
+        <f>'sensi_speed cs'!C47</f>
+        <v>18</v>
+      </c>
+      <c r="N29" s="34">
+        <f>'sensi_speed cs'!D47</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O29" s="34">
+        <f>'sensi_speed cs'!E47</f>
+        <v>6.4227999999999996</v>
+      </c>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34">
+        <f>'sensi_speed cs'!F47</f>
+        <v>9</v>
+      </c>
+      <c r="R29" s="34">
+        <f>'sensi_speed cs'!G47</f>
+        <v>12</v>
+      </c>
+      <c r="S29" s="34">
+        <f>'sensi_speed cs'!H47</f>
+        <v>8.2928999999999995</v>
+      </c>
+      <c r="T29" s="39">
+        <f>'sensi_speed cs'!I47</f>
+        <v>0.22550615586827286</v>
+      </c>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7">
+        <f>'sensi_speed cs'!K47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J30" s="40" t="str">
+        <f>'sensi_speed cs'!A51</f>
+        <v>mu1</v>
+      </c>
+      <c r="K30" s="41">
+        <f>'sensi_speed cs'!A52</f>
+        <v>0.2</v>
+      </c>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41">
+        <f>'sensi_speed cs'!C52</f>
+        <v>12</v>
+      </c>
+      <c r="N30" s="41">
+        <f>'sensi_speed cs'!D52</f>
+        <v>0.6</v>
+      </c>
+      <c r="O30" s="41">
+        <f>'sensi_speed cs'!E52</f>
+        <v>5.9827000000000004</v>
+      </c>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41">
+        <f>'sensi_speed cs'!F52</f>
+        <v>10</v>
+      </c>
+      <c r="R30" s="41">
+        <f>'sensi_speed cs'!G52</f>
+        <v>8</v>
+      </c>
+      <c r="S30" s="41">
+        <f>'sensi_speed cs'!H52</f>
+        <v>7.4097</v>
+      </c>
+      <c r="T30" s="42">
+        <f>'sensi_speed cs'!I52</f>
+        <v>0.19258539482030307</v>
+      </c>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7">
+        <f>'sensi_speed cs'!K52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J31" s="35"/>
+      <c r="K31" s="44">
+        <f>'sensi_speed cs'!A53</f>
+        <v>0.4</v>
+      </c>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44">
+        <f>'sensi_speed cs'!C53</f>
+        <v>18</v>
+      </c>
+      <c r="N31" s="44">
+        <f>'sensi_speed cs'!D53</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O31" s="44">
+        <f>'sensi_speed cs'!E53</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44">
+        <f>'sensi_speed cs'!F53</f>
+        <v>9</v>
+      </c>
+      <c r="R31" s="44">
+        <f>'sensi_speed cs'!G53</f>
+        <v>12</v>
+      </c>
+      <c r="S31" s="44">
+        <f>'sensi_speed cs'!H53</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T31" s="45">
+        <f>'sensi_speed cs'!I53</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7">
+        <f>'sensi_speed cs'!K53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J32" s="35"/>
+      <c r="K32" s="36">
+        <f>'sensi_speed cs'!A54</f>
+        <v>0.6</v>
+      </c>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36">
+        <f>'sensi_speed cs'!C54</f>
+        <v>21</v>
+      </c>
+      <c r="N32" s="36">
+        <f>'sensi_speed cs'!D54</f>
+        <v>1.3</v>
+      </c>
+      <c r="O32" s="36">
+        <f>'sensi_speed cs'!E54</f>
+        <v>7.0849000000000002</v>
+      </c>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36">
+        <f>'sensi_speed cs'!F54</f>
+        <v>9</v>
+      </c>
+      <c r="R32" s="36">
+        <f>'sensi_speed cs'!G54</f>
+        <v>13</v>
+      </c>
+      <c r="S32" s="36">
+        <f>'sensi_speed cs'!H54</f>
+        <v>9.1378000000000004</v>
+      </c>
+      <c r="T32" s="37">
+        <f>'sensi_speed cs'!I54</f>
+        <v>0.2246602026746044</v>
+      </c>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7" t="str">
+        <f>'sensi_speed cs'!K54</f>
+        <v>退化速度越大，越需要细致的观测interval来进行时刻检测。而Model B的检测成本较高，没办法实行细致检测，导致cost rate越大。</v>
+      </c>
+    </row>
+    <row r="33" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J33" s="35"/>
+      <c r="K33" s="36">
+        <f>'sensi_speed cs'!A55</f>
+        <v>0.8</v>
+      </c>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36">
+        <f>'sensi_speed cs'!C55</f>
+        <v>24</v>
+      </c>
+      <c r="N33" s="36">
+        <f>'sensi_speed cs'!D55</f>
+        <v>1.4</v>
+      </c>
+      <c r="O33" s="36">
+        <f>'sensi_speed cs'!E55</f>
+        <v>7.3578000000000001</v>
+      </c>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36">
+        <f>'sensi_speed cs'!F55</f>
+        <v>8</v>
+      </c>
+      <c r="R33" s="36">
+        <f>'sensi_speed cs'!G55</f>
+        <v>15</v>
+      </c>
+      <c r="S33" s="36">
+        <f>'sensi_speed cs'!H55</f>
+        <v>10.007199999999999</v>
+      </c>
+      <c r="T33" s="37">
+        <f>'sensi_speed cs'!I55</f>
+        <v>0.26474938044607876</v>
+      </c>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7">
+        <f>'sensi_speed cs'!K55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J34" s="38"/>
+      <c r="K34" s="34">
+        <f>'sensi_speed cs'!A56</f>
+        <v>1</v>
+      </c>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34">
+        <f>'sensi_speed cs'!C56</f>
+        <v>29</v>
+      </c>
+      <c r="N34" s="34">
+        <f>'sensi_speed cs'!D56</f>
+        <v>2.6</v>
+      </c>
+      <c r="O34" s="34">
+        <f>'sensi_speed cs'!E56</f>
+        <v>7.9672999999999998</v>
+      </c>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="34">
+        <f>'sensi_speed cs'!F56</f>
+        <v>10</v>
+      </c>
+      <c r="R34" s="34">
+        <f>'sensi_speed cs'!G56</f>
+        <v>12</v>
+      </c>
+      <c r="S34" s="34">
+        <f>'sensi_speed cs'!H56</f>
+        <v>10.875299999999999</v>
+      </c>
+      <c r="T34" s="39">
+        <f>'sensi_speed cs'!I56</f>
+        <v>0.26739492243892121</v>
+      </c>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7">
+        <f>'sensi_speed cs'!K56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J35" s="40" t="str">
+        <f>'sensi_speed cs'!A61</f>
+        <v>mu2</v>
+      </c>
+      <c r="K35" s="41">
+        <f>'sensi_speed cs'!A62</f>
+        <v>2.1</v>
+      </c>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41">
+        <f>'sensi_speed cs'!C62</f>
+        <v>20</v>
+      </c>
+      <c r="N35" s="41">
+        <f>'sensi_speed cs'!D62</f>
+        <v>1</v>
+      </c>
+      <c r="O35" s="41">
+        <f>'sensi_speed cs'!E62</f>
+        <v>5.9623999999999997</v>
+      </c>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41">
+        <f>'sensi_speed cs'!F62</f>
+        <v>11</v>
+      </c>
+      <c r="R35" s="41">
+        <f>'sensi_speed cs'!G62</f>
+        <v>13</v>
+      </c>
+      <c r="S35" s="41">
+        <f>'sensi_speed cs'!H62</f>
+        <v>7.2706999999999997</v>
+      </c>
+      <c r="T35" s="42">
+        <f>'sensi_speed cs'!I62</f>
+        <v>0.17994140866766611</v>
+      </c>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7">
+        <f>'sensi_speed cs'!K62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J36" s="35"/>
+      <c r="K36" s="36">
+        <f>'sensi_speed cs'!A63</f>
+        <v>2.4</v>
+      </c>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36">
+        <f>'sensi_speed cs'!C63</f>
+        <v>20</v>
+      </c>
+      <c r="N36" s="36">
+        <f>'sensi_speed cs'!D63</f>
+        <v>1</v>
+      </c>
+      <c r="O36" s="36">
+        <f>'sensi_speed cs'!E63</f>
+        <v>6.2030000000000003</v>
+      </c>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36">
+        <f>'sensi_speed cs'!F63</f>
+        <v>10</v>
+      </c>
+      <c r="R36" s="36">
+        <f>'sensi_speed cs'!G63</f>
+        <v>12</v>
+      </c>
+      <c r="S36" s="36">
+        <f>'sensi_speed cs'!H63</f>
+        <v>7.8150000000000004</v>
+      </c>
+      <c r="T36" s="37">
+        <f>'sensi_speed cs'!I63</f>
+        <v>0.20626999360204734</v>
+      </c>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7">
+        <f>'sensi_speed cs'!K63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J37" s="35"/>
+      <c r="K37" s="44">
+        <f>'sensi_speed cs'!A64</f>
+        <v>2.7</v>
+      </c>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44">
+        <f>'sensi_speed cs'!C64</f>
+        <v>18</v>
+      </c>
+      <c r="N37" s="44">
+        <f>'sensi_speed cs'!D64</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O37" s="44">
+        <f>'sensi_speed cs'!E64</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44">
+        <f>'sensi_speed cs'!F64</f>
+        <v>9</v>
+      </c>
+      <c r="R37" s="44">
+        <f>'sensi_speed cs'!G64</f>
+        <v>12</v>
+      </c>
+      <c r="S37" s="44">
+        <f>'sensi_speed cs'!H64</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T37" s="45">
+        <f>'sensi_speed cs'!I64</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7" t="str">
+        <f>'sensi_speed cs'!K64</f>
+        <v>同样是检测成本过高的问题</v>
+      </c>
+    </row>
+    <row r="38" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J38" s="35"/>
+      <c r="K38" s="36">
+        <f>'sensi_speed cs'!A65</f>
+        <v>3</v>
+      </c>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36">
+        <f>'sensi_speed cs'!C65</f>
+        <v>19</v>
+      </c>
+      <c r="N38" s="36">
+        <f>'sensi_speed cs'!D65</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O38" s="36">
+        <f>'sensi_speed cs'!E65</f>
+        <v>6.6249000000000002</v>
+      </c>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="36">
+        <f>'sensi_speed cs'!F65</f>
+        <v>8</v>
+      </c>
+      <c r="R38" s="36">
+        <f>'sensi_speed cs'!G65</f>
+        <v>12</v>
+      </c>
+      <c r="S38" s="36">
+        <f>'sensi_speed cs'!H65</f>
+        <v>8.8216000000000001</v>
+      </c>
+      <c r="T38" s="37">
+        <f>'sensi_speed cs'!I65</f>
+        <v>0.24901378434751065</v>
+      </c>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7">
+        <f>'sensi_speed cs'!K65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J39" s="38"/>
+      <c r="K39" s="34">
+        <f>'sensi_speed cs'!A66</f>
+        <v>3.3</v>
+      </c>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34">
+        <f>'sensi_speed cs'!C66</f>
+        <v>18</v>
+      </c>
+      <c r="N39" s="34">
+        <f>'sensi_speed cs'!D66</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O39" s="34">
+        <f>'sensi_speed cs'!E66</f>
+        <v>6.7849000000000004</v>
+      </c>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34">
+        <f>'sensi_speed cs'!F66</f>
+        <v>7</v>
+      </c>
+      <c r="R39" s="34">
+        <f>'sensi_speed cs'!G66</f>
+        <v>13</v>
+      </c>
+      <c r="S39" s="34">
+        <f>'sensi_speed cs'!H66</f>
+        <v>9.3912999999999993</v>
+      </c>
+      <c r="T39" s="39">
+        <f>'sensi_speed cs'!I66</f>
+        <v>0.27753346182104704</v>
+      </c>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7">
+        <f>'sensi_speed cs'!K66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J40" s="40" t="str">
+        <f>'sensi_speed cs'!A70</f>
+        <v>eta</v>
+      </c>
+      <c r="K40" s="41">
+        <f>'sensi_speed cs'!A71</f>
+        <v>26</v>
+      </c>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41">
+        <f>'sensi_speed cs'!C71</f>
+        <v>15</v>
+      </c>
+      <c r="N40" s="41">
+        <f>'sensi_speed cs'!D71</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O40" s="41">
+        <f>'sensi_speed cs'!E71</f>
+        <v>7.5206</v>
+      </c>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="41">
+        <f>'sensi_speed cs'!F71</f>
+        <v>9</v>
+      </c>
+      <c r="R40" s="41">
+        <f>'sensi_speed cs'!G71</f>
+        <v>11</v>
+      </c>
+      <c r="S40" s="41">
+        <f>'sensi_speed cs'!H71</f>
+        <v>8.9542999999999999</v>
+      </c>
+      <c r="T40" s="42">
+        <f>'sensi_speed cs'!I71</f>
+        <v>0.16011301832639066</v>
+      </c>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7">
+        <f>'sensi_speed cs'!K71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J41" s="35"/>
+      <c r="K41" s="36">
+        <f>'sensi_speed cs'!A72</f>
+        <v>30</v>
+      </c>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36">
+        <f>'sensi_speed cs'!C72</f>
+        <v>18</v>
+      </c>
+      <c r="N41" s="36">
+        <f>'sensi_speed cs'!D72</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O41" s="36">
+        <f>'sensi_speed cs'!E72</f>
+        <v>6.8738999999999999</v>
+      </c>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36">
+        <f>'sensi_speed cs'!F72</f>
+        <v>9</v>
+      </c>
+      <c r="R41" s="36">
+        <f>'sensi_speed cs'!G72</f>
+        <v>11</v>
+      </c>
+      <c r="S41" s="36">
+        <f>'sensi_speed cs'!H72</f>
+        <v>8.6221999999999994</v>
+      </c>
+      <c r="T41" s="37">
+        <f>'sensi_speed cs'!I72</f>
+        <v>0.20276727517338958</v>
+      </c>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7" t="str">
+        <f>'sensi_speed cs'!K72</f>
+        <v>检测成本，defect时间越靠后，MI无效开销越多</v>
+      </c>
+    </row>
+    <row r="42" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J42" s="35"/>
+      <c r="K42" s="44">
+        <f>'sensi_speed cs'!A73</f>
+        <v>34</v>
+      </c>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44">
+        <f>'sensi_speed cs'!C73</f>
+        <v>18</v>
+      </c>
+      <c r="N42" s="44">
+        <f>'sensi_speed cs'!D73</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O42" s="44">
+        <f>'sensi_speed cs'!E73</f>
+        <v>6.4233000000000002</v>
+      </c>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44">
+        <f>'sensi_speed cs'!F73</f>
+        <v>9</v>
+      </c>
+      <c r="R42" s="44">
+        <f>'sensi_speed cs'!G73</f>
+        <v>12</v>
+      </c>
+      <c r="S42" s="44">
+        <f>'sensi_speed cs'!H73</f>
+        <v>8.3257999999999992</v>
+      </c>
+      <c r="T42" s="45">
+        <f>'sensi_speed cs'!I73</f>
+        <v>0.22850656993922497</v>
+      </c>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7">
+        <f>'sensi_speed cs'!K73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J43" s="35"/>
+      <c r="K43" s="36">
+        <f>'sensi_speed cs'!A74</f>
+        <v>38</v>
+      </c>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36">
+        <f>'sensi_speed cs'!C74</f>
+        <v>18</v>
+      </c>
+      <c r="N43" s="36">
+        <f>'sensi_speed cs'!D74</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O43" s="36">
+        <f>'sensi_speed cs'!E74</f>
+        <v>6.0797999999999996</v>
+      </c>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="36">
+        <f>'sensi_speed cs'!F74</f>
+        <v>9</v>
+      </c>
+      <c r="R43" s="36">
+        <f>'sensi_speed cs'!G74</f>
+        <v>13</v>
+      </c>
+      <c r="S43" s="36">
+        <f>'sensi_speed cs'!H74</f>
+        <v>8.1298999999999992</v>
+      </c>
+      <c r="T43" s="37">
+        <f>'sensi_speed cs'!I74</f>
+        <v>0.25216792334469057</v>
+      </c>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7">
+        <f>'sensi_speed cs'!K74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J44" s="38"/>
+      <c r="K44" s="34">
+        <f>'sensi_speed cs'!A75</f>
+        <v>42</v>
+      </c>
+      <c r="L44" s="34"/>
+      <c r="M44" s="34">
+        <f>'sensi_speed cs'!C75</f>
+        <v>18</v>
+      </c>
+      <c r="N44" s="34">
+        <f>'sensi_speed cs'!D75</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O44" s="34">
+        <f>'sensi_speed cs'!E75</f>
+        <v>5.8022</v>
+      </c>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34">
+        <f>'sensi_speed cs'!F75</f>
+        <v>9</v>
+      </c>
+      <c r="R44" s="34">
+        <f>'sensi_speed cs'!G75</f>
+        <v>13</v>
+      </c>
+      <c r="S44" s="34">
+        <f>'sensi_speed cs'!H75</f>
+        <v>7.9333999999999998</v>
+      </c>
+      <c r="T44" s="39">
+        <f>'sensi_speed cs'!I75</f>
+        <v>0.26863639801346206</v>
+      </c>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7">
+        <f>'sensi_speed cs'!K75</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="14">
+    <mergeCell ref="J25:J29"/>
+    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="J35:J39"/>
+    <mergeCell ref="J40:J44"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="J5:J9"/>
+    <mergeCell ref="J10:J14"/>
+    <mergeCell ref="J15:J19"/>
+    <mergeCell ref="J20:J24"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1386,20 +3260,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27BF723-D6DC-4608-ABE2-E81C591742E9}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="R63" sqref="R63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="19.58203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.58203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
@@ -1410,181 +3283,178 @@
         <v>11</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
       <c r="D2">
-        <v>21</v>
-      </c>
-      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="22">
+      <c r="E2" s="22">
         <v>5.8662999999999998</v>
       </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
       <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2" s="22">
+        <v>12</v>
+      </c>
+      <c r="H2" s="22">
         <v>7.9919000000000002</v>
       </c>
-      <c r="J2" s="1">
-        <f>(I2-F2)/I2</f>
+      <c r="I2" s="1">
+        <f>(H2-E2)/H2</f>
         <v>0.265969293910084</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>5</v>
       </c>
       <c r="B3">
         <v>6</v>
       </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
       <c r="D3">
-        <v>18</v>
-      </c>
-      <c r="E3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F3" s="22">
+      <c r="E3" s="22">
         <v>6.4233000000000002</v>
       </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
       <c r="G3">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3" s="28">
+        <v>12</v>
+      </c>
+      <c r="H3" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J6" si="0">(I3-F3)/I3</f>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I6" si="0">(H3-E3)/H3</f>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
       <c r="D4">
-        <v>19</v>
-      </c>
-      <c r="E4">
         <v>1.2</v>
       </c>
-      <c r="F4" s="22">
+      <c r="E4" s="22">
         <v>6.8905000000000003</v>
       </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
       <c r="G4">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4" s="22">
+        <v>12</v>
+      </c>
+      <c r="H4" s="22">
         <v>8.6296999999999997</v>
       </c>
-      <c r="J4" s="1">
+      <c r="I4" s="1">
         <f t="shared" si="0"/>
         <v>0.20153655399376566</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
       <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="22">
+      <c r="E5" s="22">
         <v>7.3307000000000002</v>
       </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
       <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5" s="23">
+        <v>12</v>
+      </c>
+      <c r="H5" s="23">
         <v>8.9352</v>
       </c>
-      <c r="J5" s="1">
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>0.17957068672217744</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
       <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="22">
+      <c r="E6" s="22">
         <v>7.7404000000000002</v>
       </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
       <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6" s="22">
+        <v>12</v>
+      </c>
+      <c r="H6" s="22">
         <v>9.3028999999999993</v>
       </c>
-      <c r="J6" s="1">
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>0.16795837857012322</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -1595,58 +3465,55 @@
         <v>11</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="I11" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
       <c r="D12">
-        <v>18</v>
-      </c>
-      <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="22">
+      <c r="E12" s="22">
         <v>6.4054000000000002</v>
       </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
       <c r="G12">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>12</v>
-      </c>
-      <c r="I12" s="22">
+        <v>12</v>
+      </c>
+      <c r="H12" s="22">
         <v>8.0942000000000007</v>
       </c>
-      <c r="J12" s="1">
-        <f>(I12-F12)/I12</f>
+      <c r="I12" s="1">
+        <f>(H12-E12)/H12</f>
         <v>0.20864322601368887</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>15</v>
       </c>
@@ -1654,122 +3521,122 @@
         <f>B3</f>
         <v>6</v>
       </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
       <c r="D13">
-        <v>18</v>
-      </c>
-      <c r="E13">
+        <f>D3</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E13" s="22">
         <f>E3</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F13" s="22">
-        <f>F3</f>
         <v>6.4233000000000002</v>
       </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
       <c r="G13">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>12</v>
-      </c>
-      <c r="I13" s="28">
+        <v>12</v>
+      </c>
+      <c r="H13" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" ref="J13:J16" si="1">(I13-F13)/I13</f>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:I16" si="1">(H13-E13)/H13</f>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
       <c r="D14">
-        <v>18</v>
-      </c>
-      <c r="E14">
         <v>1.3</v>
       </c>
-      <c r="F14" s="22">
+      <c r="E14" s="22">
         <v>6.4127000000000001</v>
       </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
       <c r="G14">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>12</v>
-      </c>
-      <c r="I14" s="22">
+        <v>12</v>
+      </c>
+      <c r="H14" s="22">
         <v>8.5197000000000003</v>
       </c>
-      <c r="J14" s="1">
+      <c r="I14" s="1">
         <f t="shared" si="1"/>
         <v>0.24730917755320025</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>25</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
       <c r="D15">
-        <v>18</v>
-      </c>
-      <c r="E15">
         <v>0.9</v>
       </c>
-      <c r="F15" s="22">
+      <c r="E15" s="22">
         <v>6.4028999999999998</v>
       </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
       <c r="G15">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>12</v>
-      </c>
-      <c r="I15" s="22">
+        <v>12</v>
+      </c>
+      <c r="H15" s="22">
         <v>8.8023000000000007</v>
       </c>
-      <c r="J15" s="1">
+      <c r="I15" s="1">
         <f t="shared" si="1"/>
         <v>0.27258784635833821</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>30</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
       <c r="D16">
-        <v>18</v>
-      </c>
-      <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="22">
+      <c r="E16" s="22">
         <v>6.4105999999999996</v>
       </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
       <c r="G16">
-        <v>9</v>
-      </c>
-      <c r="H16">
-        <v>12</v>
-      </c>
-      <c r="I16" s="22">
+        <v>12</v>
+      </c>
+      <c r="H16" s="22">
         <v>9.0268999999999995</v>
       </c>
-      <c r="J16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="1"/>
         <v>0.28983371921700696</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>16</v>
       </c>
@@ -1780,88 +3647,85 @@
         <v>11</v>
       </c>
       <c r="D22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="24" t="s">
+      <c r="H22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="I22" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
+      <c r="C23">
+        <v>18</v>
+      </c>
       <c r="D23">
-        <v>18</v>
-      </c>
-      <c r="E23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F23" s="22">
+      <c r="E23" s="22">
         <v>3.6124999999999998</v>
       </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
       <c r="G23">
-        <v>9</v>
-      </c>
-      <c r="H23">
         <v>11</v>
       </c>
-      <c r="I23" s="22">
+      <c r="H23" s="22">
         <v>5.0346000000000002</v>
       </c>
-      <c r="J23" s="1">
-        <f>(I23-F23)/I23</f>
+      <c r="I23" s="1">
+        <f>(H23-E23)/H23</f>
         <v>0.28246533984825017</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>150</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
+      <c r="C24">
+        <v>18</v>
+      </c>
       <c r="D24">
-        <v>18</v>
-      </c>
-      <c r="E24">
         <v>0.8</v>
       </c>
-      <c r="F24" s="22">
+      <c r="E24" s="22">
         <v>5.0114000000000001</v>
       </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
       <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="H24">
-        <v>9</v>
-      </c>
-      <c r="I24" s="22">
+        <v>9</v>
+      </c>
+      <c r="H24" s="22">
         <v>6.7560000000000002</v>
       </c>
-      <c r="J24" s="1">
-        <f t="shared" ref="J24:J27" si="2">(I24-F24)/I24</f>
+      <c r="I24" s="1">
+        <f t="shared" ref="I24:I27" si="2">(H24-E24)/H24</f>
         <v>0.25822972172883363</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>200</v>
       </c>
@@ -1869,93 +3733,93 @@
         <f>B3</f>
         <v>6</v>
       </c>
+      <c r="C25">
+        <f>C3</f>
+        <v>18</v>
+      </c>
       <c r="D25">
         <f>D3</f>
-        <v>18</v>
-      </c>
-      <c r="E25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E25" s="22">
         <f>E3</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F25" s="22">
-        <f>F3</f>
         <v>6.4233000000000002</v>
       </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
       <c r="G25">
-        <v>9</v>
-      </c>
-      <c r="H25">
-        <v>12</v>
-      </c>
-      <c r="I25" s="28">
+        <v>12</v>
+      </c>
+      <c r="H25" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="2"/>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>250</v>
       </c>
       <c r="B26">
         <v>6</v>
       </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
       <c r="D26">
-        <v>18</v>
-      </c>
-      <c r="E26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F26" s="22">
+      <c r="E26" s="22">
         <v>7.8053999999999997</v>
       </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
       <c r="G26">
-        <v>9</v>
-      </c>
-      <c r="H26">
-        <v>12</v>
-      </c>
-      <c r="I26" s="22">
+        <v>12</v>
+      </c>
+      <c r="H26" s="22">
         <v>10.026400000000001</v>
       </c>
-      <c r="J26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="2"/>
         <v>0.22151519987233712</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>300</v>
       </c>
       <c r="B27">
         <v>6</v>
       </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
       <c r="D27">
-        <v>19</v>
-      </c>
-      <c r="E27">
         <v>1.4</v>
       </c>
-      <c r="F27" s="22">
+      <c r="E27" s="22">
         <v>9.1647999999999996</v>
       </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
       <c r="G27">
-        <v>9</v>
-      </c>
-      <c r="H27">
         <v>13</v>
       </c>
-      <c r="I27" s="22">
+      <c r="H27" s="22">
         <v>11.72</v>
       </c>
-      <c r="J27" s="1">
+      <c r="I27" s="1">
         <f t="shared" si="2"/>
         <v>0.21802047781569975</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>17</v>
       </c>
@@ -1966,58 +3830,55 @@
         <v>11</v>
       </c>
       <c r="D33" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="I33" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1500</v>
       </c>
       <c r="B34">
         <v>6</v>
       </c>
+      <c r="C34">
+        <v>18</v>
+      </c>
       <c r="D34">
-        <v>18</v>
-      </c>
-      <c r="E34">
         <v>0.9</v>
       </c>
-      <c r="F34" s="22">
+      <c r="E34" s="22">
         <v>6.4108999999999998</v>
       </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
       <c r="G34">
-        <v>9</v>
-      </c>
-      <c r="H34">
         <v>13</v>
       </c>
-      <c r="I34" s="22">
+      <c r="H34" s="22">
         <v>8.2538</v>
       </c>
-      <c r="J34" s="1">
-        <f>(I34-F34)/I34</f>
+      <c r="I34" s="1">
+        <f>(H34-E34)/H34</f>
         <v>0.22327897453294243</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
         <v>2000</v>
       </c>
@@ -2026,131 +3887,127 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:E35" si="3">C3</f>
-        <v>0</v>
+        <f t="shared" ref="C35:D35" si="3">C3</f>
+        <v>18</v>
       </c>
       <c r="D35">
         <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="3"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F35" s="22">
-        <f>F3</f>
+      <c r="E35" s="22">
+        <f>E3</f>
         <v>6.4233000000000002</v>
       </c>
+      <c r="F35">
+        <v>9</v>
+      </c>
       <c r="G35">
-        <v>9</v>
-      </c>
-      <c r="H35">
-        <v>12</v>
-      </c>
-      <c r="I35" s="28">
+        <v>12</v>
+      </c>
+      <c r="H35" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J35" s="1">
-        <f t="shared" ref="J35:J38" si="4">(I35-F35)/I35</f>
+      <c r="I35" s="1">
+        <f t="shared" ref="I35:I38" si="4">(H35-E35)/H35</f>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>2500</v>
       </c>
       <c r="B36">
         <v>6</v>
       </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
       <c r="D36">
-        <v>18</v>
-      </c>
-      <c r="E36">
         <v>0.9</v>
       </c>
-      <c r="F36" s="22">
+      <c r="E36" s="22">
         <v>6.4051999999999998</v>
       </c>
+      <c r="F36">
+        <v>9</v>
+      </c>
       <c r="G36">
-        <v>9</v>
-      </c>
-      <c r="H36">
-        <v>12</v>
-      </c>
-      <c r="I36" s="22">
+        <v>12</v>
+      </c>
+      <c r="H36" s="22">
         <v>8.3809000000000005</v>
       </c>
-      <c r="J36" s="1">
+      <c r="I36" s="1">
         <f t="shared" si="4"/>
         <v>0.23573840518321429</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3000</v>
       </c>
       <c r="B37">
         <v>6</v>
       </c>
+      <c r="C37">
+        <v>18</v>
+      </c>
       <c r="D37">
-        <v>18</v>
-      </c>
-      <c r="E37">
         <v>1.4</v>
       </c>
-      <c r="F37" s="22">
+      <c r="E37" s="22">
         <v>6.4229000000000003</v>
       </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
       <c r="G37">
-        <v>9</v>
-      </c>
-      <c r="H37">
-        <v>12</v>
-      </c>
-      <c r="I37" s="22">
+        <v>12</v>
+      </c>
+      <c r="H37" s="22">
         <v>8.4442000000000004</v>
       </c>
-      <c r="J37" s="1">
+      <c r="I37" s="1">
         <f t="shared" si="4"/>
         <v>0.23937140285639846</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3500</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
       <c r="D38">
-        <v>18</v>
-      </c>
-      <c r="E38">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F38" s="22">
+      <c r="E38" s="22">
         <v>6.4227999999999996</v>
       </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
       <c r="G38">
-        <v>9</v>
-      </c>
-      <c r="H38">
         <v>11</v>
       </c>
-      <c r="I38" s="22">
+      <c r="H38" s="22">
         <v>8.4097000000000008</v>
       </c>
-      <c r="J38" s="1">
+      <c r="I38" s="1">
         <f t="shared" si="4"/>
         <v>0.23626288690440814</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F39" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E39" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>47</v>
       </c>
@@ -2161,58 +4018,55 @@
         <v>11</v>
       </c>
       <c r="D42" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="24" t="s">
+      <c r="H42" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="I42" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>20</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
+      <c r="C43">
+        <v>18</v>
+      </c>
       <c r="D43">
-        <v>18</v>
-      </c>
-      <c r="E43">
         <v>0.9</v>
       </c>
-      <c r="F43" s="22">
+      <c r="E43" s="22">
         <v>6.4108999999999998</v>
       </c>
+      <c r="F43">
+        <v>9</v>
+      </c>
       <c r="G43">
-        <v>9</v>
-      </c>
-      <c r="H43">
         <v>13</v>
       </c>
-      <c r="I43" s="22">
+      <c r="H43" s="22">
         <v>8.3396000000000008</v>
       </c>
-      <c r="J43" s="1">
-        <f>(I43-F43)/I43</f>
+      <c r="I43" s="1">
+        <f>(H43-E43)/H43</f>
         <v>0.23127008489615819</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="26">
         <v>30</v>
       </c>
@@ -2221,128 +4075,123 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:E44" si="5">C12</f>
-        <v>0</v>
+        <f t="shared" ref="C44:D44" si="5">C12</f>
+        <v>18</v>
       </c>
       <c r="D44">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="F44" s="22">
-        <f>F12</f>
+      <c r="E44" s="22">
+        <f>E12</f>
         <v>6.4054000000000002</v>
       </c>
+      <c r="F44">
+        <v>9</v>
+      </c>
       <c r="G44">
-        <v>9</v>
-      </c>
-      <c r="H44">
-        <v>12</v>
-      </c>
-      <c r="I44" s="25">
+        <v>12</v>
+      </c>
+      <c r="H44" s="25">
         <v>8.3114000000000008</v>
       </c>
-      <c r="J44" s="1">
-        <f t="shared" ref="J44:J47" si="6">(I44-F44)/I44</f>
+      <c r="I44" s="1">
+        <f t="shared" ref="I44:I47" si="6">(H44-E44)/H44</f>
         <v>0.22932357966166955</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="27">
         <v>40</v>
       </c>
       <c r="B45" s="19">
         <v>6</v>
       </c>
-      <c r="C45" s="19"/>
+      <c r="C45" s="19">
+        <v>18</v>
+      </c>
       <c r="D45" s="19">
-        <v>18</v>
-      </c>
-      <c r="E45" s="19">
         <v>1</v>
       </c>
-      <c r="F45" s="22">
-        <f>F13</f>
+      <c r="E45" s="22">
+        <f>E13</f>
         <v>6.4233000000000002</v>
       </c>
+      <c r="F45" s="19">
+        <v>9</v>
+      </c>
       <c r="G45" s="19">
-        <v>9</v>
-      </c>
-      <c r="H45" s="19">
-        <v>12</v>
-      </c>
-      <c r="I45" s="28">
+        <v>12</v>
+      </c>
+      <c r="H45" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J45" s="29">
+      <c r="I45" s="29">
         <f t="shared" si="6"/>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>50</v>
       </c>
       <c r="B46">
         <v>6</v>
       </c>
+      <c r="C46">
+        <v>18</v>
+      </c>
       <c r="D46">
-        <v>18</v>
-      </c>
-      <c r="E46">
         <v>1.4</v>
       </c>
-      <c r="F46" s="22">
+      <c r="E46" s="22">
         <v>6.4229000000000003</v>
       </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
       <c r="G46">
-        <v>9</v>
-      </c>
-      <c r="H46">
-        <v>12</v>
-      </c>
-      <c r="I46" s="22">
+        <v>12</v>
+      </c>
+      <c r="H46" s="22">
         <v>8.3124000000000002</v>
       </c>
-      <c r="J46" s="1">
+      <c r="I46" s="1">
         <f t="shared" si="6"/>
         <v>0.22731100524517586</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="26">
         <v>60</v>
       </c>
       <c r="B47">
         <v>6</v>
       </c>
+      <c r="C47">
+        <v>18</v>
+      </c>
       <c r="D47">
-        <v>18</v>
-      </c>
-      <c r="E47">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F47" s="22">
+      <c r="E47" s="22">
         <v>6.4227999999999996</v>
       </c>
+      <c r="F47">
+        <v>9</v>
+      </c>
       <c r="G47">
-        <v>9</v>
-      </c>
-      <c r="H47">
-        <v>12</v>
-      </c>
-      <c r="I47" s="22">
+        <v>12</v>
+      </c>
+      <c r="H47" s="22">
         <v>8.2928999999999995</v>
       </c>
-      <c r="J47" s="1">
+      <c r="I47" s="1">
         <f t="shared" si="6"/>
         <v>0.22550615586827286</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>50</v>
       </c>
@@ -2353,181 +4202,178 @@
         <v>11</v>
       </c>
       <c r="D51" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" s="24" t="s">
+      <c r="H51" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J51" s="18" t="s">
+      <c r="I51" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0.2</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
       <c r="D52">
-        <v>12</v>
-      </c>
-      <c r="E52">
         <v>0.6</v>
       </c>
-      <c r="F52" s="22">
+      <c r="E52" s="22">
         <v>5.9827000000000004</v>
       </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
       <c r="G52">
-        <v>10</v>
-      </c>
-      <c r="H52">
         <v>8</v>
       </c>
-      <c r="I52" s="22">
+      <c r="H52" s="22">
         <v>7.4097</v>
       </c>
-      <c r="J52" s="1">
-        <f>(I52-F52)/I52</f>
+      <c r="I52" s="1">
+        <f>(H52-E52)/H52</f>
         <v>0.19258539482030307</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="21">
         <v>0.4</v>
       </c>
       <c r="B53">
         <v>6</v>
       </c>
+      <c r="C53">
+        <v>18</v>
+      </c>
       <c r="D53">
-        <v>18</v>
-      </c>
-      <c r="E53">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F53" s="22">
+      <c r="E53" s="22">
         <v>6.4233000000000002</v>
       </c>
+      <c r="F53">
+        <v>9</v>
+      </c>
       <c r="G53">
-        <v>9</v>
-      </c>
-      <c r="H53">
-        <v>12</v>
-      </c>
-      <c r="I53" s="28">
+        <v>12</v>
+      </c>
+      <c r="H53" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J53" s="1">
-        <f t="shared" ref="J53:J56" si="7">(I53-F53)/I53</f>
+      <c r="I53" s="1">
+        <f t="shared" ref="I53:I56" si="7">(H53-E53)/H53</f>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="17">
         <v>0.6</v>
       </c>
       <c r="B54">
         <v>5</v>
       </c>
+      <c r="C54">
+        <v>21</v>
+      </c>
       <c r="D54">
-        <v>21</v>
-      </c>
-      <c r="E54">
         <v>1.3</v>
       </c>
-      <c r="F54" s="22">
+      <c r="E54" s="22">
         <v>7.0849000000000002</v>
       </c>
+      <c r="F54">
+        <v>9</v>
+      </c>
       <c r="G54">
-        <v>9</v>
-      </c>
-      <c r="H54">
         <v>13</v>
       </c>
-      <c r="I54" s="22">
+      <c r="H54" s="22">
         <v>9.1378000000000004</v>
       </c>
-      <c r="J54" s="1">
+      <c r="I54" s="1">
         <f t="shared" si="7"/>
         <v>0.2246602026746044</v>
       </c>
-      <c r="L54" t="s">
+      <c r="K54" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0.8</v>
       </c>
       <c r="B55">
         <v>6</v>
       </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
       <c r="D55">
-        <v>24</v>
-      </c>
-      <c r="E55">
         <v>1.4</v>
       </c>
-      <c r="F55" s="22">
+      <c r="E55" s="22">
         <v>7.3578000000000001</v>
       </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
       <c r="G55">
-        <v>8</v>
-      </c>
-      <c r="H55">
         <v>15</v>
       </c>
-      <c r="I55" s="22">
+      <c r="H55" s="22">
         <v>10.007199999999999</v>
       </c>
-      <c r="J55" s="1">
+      <c r="I55" s="1">
         <f t="shared" si="7"/>
         <v>0.26474938044607876</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="26">
         <v>1</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
+      <c r="C56">
+        <v>29</v>
+      </c>
       <c r="D56">
-        <v>29</v>
-      </c>
-      <c r="E56">
         <v>2.6</v>
       </c>
-      <c r="F56" s="22">
+      <c r="E56" s="22">
         <v>7.9672999999999998</v>
       </c>
+      <c r="F56">
+        <v>10</v>
+      </c>
       <c r="G56">
-        <v>10</v>
-      </c>
-      <c r="H56">
-        <v>12</v>
-      </c>
-      <c r="I56" s="22">
+        <v>12</v>
+      </c>
+      <c r="H56" s="22">
         <v>10.875299999999999</v>
       </c>
-      <c r="J56" s="1">
+      <c r="I56" s="1">
         <f t="shared" si="7"/>
         <v>0.26739492243892121</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>51</v>
       </c>
@@ -2538,181 +4384,178 @@
         <v>11</v>
       </c>
       <c r="D61" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" s="24" t="s">
+      <c r="H61" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J61" s="18" t="s">
+      <c r="I61" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2.1</v>
       </c>
       <c r="B62">
         <v>7</v>
       </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
       <c r="D62">
-        <v>20</v>
-      </c>
-      <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" s="22">
+      <c r="E62" s="22">
         <v>5.9623999999999997</v>
       </c>
+      <c r="F62">
+        <v>11</v>
+      </c>
       <c r="G62">
-        <v>11</v>
-      </c>
-      <c r="H62">
         <v>13</v>
       </c>
-      <c r="I62" s="22">
+      <c r="H62" s="22">
         <v>7.2706999999999997</v>
       </c>
-      <c r="J62" s="1">
-        <f>(I62-F62)/I62</f>
+      <c r="I62" s="1">
+        <f>(H62-E62)/H62</f>
         <v>0.17994140866766611</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="17">
         <v>2.4</v>
       </c>
       <c r="B63">
         <v>6</v>
       </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
       <c r="D63">
-        <v>20</v>
-      </c>
-      <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" s="22">
+      <c r="E63" s="22">
         <v>6.2030000000000003</v>
       </c>
+      <c r="F63">
+        <v>10</v>
+      </c>
       <c r="G63">
-        <v>10</v>
-      </c>
-      <c r="H63">
-        <v>12</v>
-      </c>
-      <c r="I63" s="28">
+        <v>12</v>
+      </c>
+      <c r="H63" s="28">
         <v>7.8150000000000004</v>
       </c>
-      <c r="J63" s="1">
-        <f t="shared" ref="J63:J66" si="8">(I63-F63)/I63</f>
+      <c r="I63" s="1">
+        <f t="shared" ref="I63:I66" si="8">(H63-E63)/H63</f>
         <v>0.20626999360204734</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>2.7</v>
       </c>
       <c r="B64">
         <v>6</v>
       </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
       <c r="D64">
-        <v>18</v>
-      </c>
-      <c r="E64">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F64" s="22">
+      <c r="E64" s="22">
         <v>6.4233000000000002</v>
       </c>
+      <c r="F64">
+        <v>9</v>
+      </c>
       <c r="G64">
-        <v>9</v>
-      </c>
-      <c r="H64">
-        <v>12</v>
-      </c>
-      <c r="I64" s="28">
+        <v>12</v>
+      </c>
+      <c r="H64" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J64" s="1">
+      <c r="I64" s="1">
         <f t="shared" si="8"/>
         <v>0.22850656993922497</v>
       </c>
-      <c r="L64" t="s">
+      <c r="K64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
       <c r="B65">
         <v>5</v>
       </c>
+      <c r="C65">
+        <v>19</v>
+      </c>
       <c r="D65">
-        <v>19</v>
-      </c>
-      <c r="E65">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F65" s="22">
+      <c r="E65" s="22">
         <v>6.6249000000000002</v>
       </c>
+      <c r="F65">
+        <v>8</v>
+      </c>
       <c r="G65">
-        <v>8</v>
-      </c>
-      <c r="H65">
-        <v>12</v>
-      </c>
-      <c r="I65" s="23">
+        <v>12</v>
+      </c>
+      <c r="H65" s="23">
         <v>8.8216000000000001</v>
       </c>
-      <c r="J65" s="1">
+      <c r="I65" s="1">
         <f t="shared" si="8"/>
         <v>0.24901378434751065</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="17">
         <v>3.3</v>
       </c>
       <c r="B66">
         <v>5</v>
       </c>
+      <c r="C66">
+        <v>18</v>
+      </c>
       <c r="D66">
-        <v>18</v>
-      </c>
-      <c r="E66">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F66" s="22">
+      <c r="E66" s="22">
         <v>6.7849000000000004</v>
       </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
       <c r="G66">
-        <v>7</v>
-      </c>
-      <c r="H66">
         <v>13</v>
       </c>
-      <c r="I66" s="22">
+      <c r="H66" s="22">
         <v>9.3912999999999993</v>
       </c>
-      <c r="J66" s="1">
+      <c r="I66" s="1">
         <f t="shared" si="8"/>
         <v>0.27753346182104704</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>52</v>
       </c>
@@ -2723,181 +4566,178 @@
         <v>11</v>
       </c>
       <c r="D70" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I70" s="24" t="s">
+      <c r="H70" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J70" s="18" t="s">
+      <c r="I70" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>26</v>
       </c>
       <c r="B71">
         <v>7</v>
       </c>
+      <c r="C71">
+        <v>15</v>
+      </c>
       <c r="D71">
-        <v>15</v>
-      </c>
-      <c r="E71">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F71" s="22">
+      <c r="E71" s="22">
         <v>7.5206</v>
       </c>
+      <c r="F71">
+        <v>9</v>
+      </c>
       <c r="G71">
-        <v>9</v>
-      </c>
-      <c r="H71">
         <v>11</v>
       </c>
-      <c r="I71" s="22">
+      <c r="H71" s="22">
         <v>8.9542999999999999</v>
       </c>
-      <c r="J71" s="1">
-        <f>(I71-F71)/I71</f>
+      <c r="I71" s="1">
+        <f>(H71-E71)/H71</f>
         <v>0.16011301832639066</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="17">
         <v>30</v>
       </c>
       <c r="B72">
         <v>6</v>
       </c>
+      <c r="C72">
+        <v>18</v>
+      </c>
       <c r="D72">
-        <v>18</v>
-      </c>
-      <c r="E72">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F72" s="22">
+      <c r="E72" s="22">
         <v>6.8738999999999999</v>
       </c>
+      <c r="F72">
+        <v>9</v>
+      </c>
       <c r="G72">
-        <v>9</v>
-      </c>
-      <c r="H72">
         <v>11</v>
       </c>
-      <c r="I72" s="28">
+      <c r="H72" s="28">
         <v>8.6221999999999994</v>
       </c>
-      <c r="J72" s="1">
-        <f t="shared" ref="J72:J75" si="9">(I72-F72)/I72</f>
+      <c r="I72" s="1">
+        <f t="shared" ref="I72:I75" si="9">(H72-E72)/H72</f>
         <v>0.20276727517338958</v>
       </c>
-      <c r="L72" t="s">
+      <c r="K72" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>34</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
+      <c r="C73">
+        <v>18</v>
+      </c>
       <c r="D73">
-        <v>18</v>
-      </c>
-      <c r="E73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F73" s="22">
+      <c r="E73" s="22">
         <v>6.4233000000000002</v>
       </c>
+      <c r="F73">
+        <v>9</v>
+      </c>
       <c r="G73">
-        <v>9</v>
-      </c>
-      <c r="H73">
-        <v>12</v>
-      </c>
-      <c r="I73" s="28">
+        <v>12</v>
+      </c>
+      <c r="H73" s="28">
         <v>8.3257999999999992</v>
       </c>
-      <c r="J73" s="1">
+      <c r="I73" s="1">
         <f t="shared" si="9"/>
         <v>0.22850656993922497</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>38</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
+      <c r="C74">
+        <v>18</v>
+      </c>
       <c r="D74">
-        <v>18</v>
-      </c>
-      <c r="E74">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F74" s="22">
+      <c r="E74" s="22">
         <v>6.0797999999999996</v>
       </c>
+      <c r="F74">
+        <v>9</v>
+      </c>
       <c r="G74">
-        <v>9</v>
-      </c>
-      <c r="H74">
         <v>13</v>
       </c>
-      <c r="I74" s="32">
+      <c r="H74" s="31">
         <v>8.1298999999999992</v>
       </c>
-      <c r="J74" s="1">
+      <c r="I74" s="1">
         <f t="shared" si="9"/>
         <v>0.25216792334469057</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="17">
         <v>42</v>
       </c>
       <c r="B75">
         <v>6</v>
       </c>
+      <c r="C75">
+        <v>18</v>
+      </c>
       <c r="D75">
-        <v>18</v>
-      </c>
-      <c r="E75">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F75" s="22">
+      <c r="E75" s="22">
         <v>5.8022</v>
       </c>
+      <c r="F75">
+        <v>9</v>
+      </c>
       <c r="G75">
-        <v>9</v>
-      </c>
-      <c r="H75">
         <v>13</v>
       </c>
-      <c r="I75" s="22">
+      <c r="H75" s="22">
         <v>7.9333999999999998</v>
       </c>
-      <c r="J75" s="1">
+      <c r="I75" s="1">
         <f t="shared" si="9"/>
         <v>0.26863639801346206</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
feat: add baysian optimization to accelerate param opt
</commit_message>
<xml_diff>
--- a/FP_result.xlsx
+++ b/FP_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy\Desktop\code_ress\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5943C704-F940-4B55-AB30-D9CD1CCEAF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E37A0-3E6E-4C04-87C8-616132519A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="64">
   <si>
     <t>FP</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -588,7 +588,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -680,17 +680,13 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -707,20 +703,23 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1418,21 +1417,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DEFD31-C20C-4FCF-BDFB-E8B3E171E50B}">
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="10" width="4.9140625" customWidth="1"/>
+    <col min="11" max="11" width="8.08203125" customWidth="1"/>
     <col min="12" max="12" width="1.25" customWidth="1"/>
-    <col min="16" max="16" width="1.25" customWidth="1"/>
-    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="13" max="15" width="5.58203125" customWidth="1"/>
+    <col min="16" max="16" width="8.08203125" customWidth="1"/>
+    <col min="17" max="17" width="1.25" customWidth="1"/>
+    <col min="18" max="19" width="5.58203125" customWidth="1"/>
+    <col min="20" max="20" width="8.08203125" customWidth="1"/>
+    <col min="21" max="21" width="7.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
@@ -1445,11 +1449,11 @@
         <v>57</v>
       </c>
       <c r="K1" s="48"/>
-      <c r="M1" s="52" t="s">
+      <c r="N1" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="11" t="s">
         <v>36</v>
@@ -1464,7 +1468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>44</v>
       </c>
@@ -1485,20 +1489,21 @@
       <c r="L3" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="46" t="s">
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="7"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
       <c r="V3" s="7"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>20</v>
       </c>
@@ -1517,33 +1522,36 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="41"/>
-      <c r="M4" s="41" t="s">
+      <c r="M4" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="O4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="P4" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41" t="s">
-        <v>10</v>
-      </c>
+      <c r="Q4" s="41"/>
       <c r="R4" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="41" t="s">
+      <c r="T4" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="T4" s="42" t="s">
+      <c r="U4" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="U4" s="7"/>
       <c r="V4" s="7"/>
-      <c r="W4" s="53"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W4" s="7"/>
+      <c r="X4" s="44"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
@@ -1559,7 +1567,7 @@
       <c r="E5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="53" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="33">
@@ -1568,38 +1576,42 @@
       </c>
       <c r="L5" s="33"/>
       <c r="M5" s="33">
+        <f>'sensi_speed cs'!B2</f>
+        <v>5</v>
+      </c>
+      <c r="N5" s="33">
         <f>'sensi_speed cs'!C2</f>
         <v>21</v>
       </c>
-      <c r="N5" s="33">
+      <c r="O5" s="33">
         <f>'sensi_speed cs'!D2</f>
         <v>1</v>
       </c>
-      <c r="O5" s="33">
+      <c r="P5" s="33">
         <f>'sensi_speed cs'!E2</f>
         <v>5.8662999999999998</v>
       </c>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33">
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33">
         <f>'sensi_speed cs'!F2</f>
         <v>9</v>
       </c>
-      <c r="R5" s="33">
+      <c r="S5" s="33">
         <f>'sensi_speed cs'!G2</f>
         <v>12</v>
       </c>
-      <c r="S5" s="33">
+      <c r="T5" s="33">
         <f>'sensi_speed cs'!H2</f>
         <v>7.9919000000000002</v>
       </c>
-      <c r="T5" s="34">
+      <c r="U5" s="34">
         <f>'sensi_speed cs'!I2</f>
         <v>0.265969293910084</v>
       </c>
-      <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-    </row>
-    <row r="6" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:24" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -1619,163 +1631,179 @@
         <f>(E4-$E$4)/E4</f>
         <v>0</v>
       </c>
-      <c r="J6" s="44"/>
+      <c r="J6" s="53"/>
       <c r="K6" s="38">
         <f>'sensi_speed cs'!A3</f>
         <v>5</v>
       </c>
       <c r="L6" s="38"/>
-      <c r="M6" s="38">
+      <c r="M6" s="33">
+        <f>'sensi_speed cs'!B3</f>
+        <v>6</v>
+      </c>
+      <c r="N6" s="38">
         <f>'sensi_speed cs'!C3</f>
         <v>18</v>
       </c>
-      <c r="N6" s="38">
+      <c r="O6" s="38">
         <f>'sensi_speed cs'!D3</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O6" s="38">
+      <c r="P6" s="38">
         <f>'sensi_speed cs'!E3</f>
         <v>6.4233000000000002</v>
       </c>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38">
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38">
         <f>'sensi_speed cs'!F3</f>
         <v>9</v>
       </c>
-      <c r="R6" s="38">
+      <c r="S6" s="38">
         <f>'sensi_speed cs'!G3</f>
         <v>12</v>
       </c>
-      <c r="S6" s="38">
+      <c r="T6" s="38">
         <f>'sensi_speed cs'!H3</f>
         <v>8.3257999999999992</v>
       </c>
-      <c r="T6" s="39">
+      <c r="U6" s="39">
         <f>'sensi_speed cs'!I3</f>
         <v>0.22850656993922497</v>
       </c>
-      <c r="U6" s="7"/>
       <c r="V6" s="7"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J7" s="44"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J7" s="53"/>
       <c r="K7" s="33">
         <f>'sensi_speed cs'!A4</f>
         <v>8</v>
       </c>
       <c r="L7" s="33"/>
       <c r="M7" s="33">
+        <f>'sensi_speed cs'!B4</f>
+        <v>6</v>
+      </c>
+      <c r="N7" s="33">
         <f>'sensi_speed cs'!C4</f>
         <v>19</v>
       </c>
-      <c r="N7" s="33">
+      <c r="O7" s="33">
         <f>'sensi_speed cs'!D4</f>
         <v>1.2</v>
       </c>
-      <c r="O7" s="33">
+      <c r="P7" s="33">
         <f>'sensi_speed cs'!E4</f>
         <v>6.8905000000000003</v>
       </c>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33">
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33">
         <f>'sensi_speed cs'!F4</f>
         <v>9</v>
       </c>
-      <c r="R7" s="33">
+      <c r="S7" s="33">
         <f>'sensi_speed cs'!G4</f>
         <v>12</v>
       </c>
-      <c r="S7" s="33">
+      <c r="T7" s="33">
         <f>'sensi_speed cs'!H4</f>
         <v>8.6296999999999997</v>
       </c>
-      <c r="T7" s="34">
+      <c r="U7" s="34">
         <f>'sensi_speed cs'!I4</f>
         <v>0.20153655399376566</v>
       </c>
-      <c r="U7" s="7"/>
       <c r="V7" s="7"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J8" s="44"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J8" s="53"/>
       <c r="K8" s="33">
         <f>'sensi_speed cs'!A5</f>
         <v>11</v>
       </c>
       <c r="L8" s="33"/>
       <c r="M8" s="33">
+        <f>'sensi_speed cs'!B5</f>
+        <v>7</v>
+      </c>
+      <c r="N8" s="33">
         <f>'sensi_speed cs'!C5</f>
         <v>16</v>
       </c>
-      <c r="N8" s="33">
+      <c r="O8" s="33">
         <f>'sensi_speed cs'!D5</f>
         <v>1</v>
       </c>
-      <c r="O8" s="33">
+      <c r="P8" s="33">
         <f>'sensi_speed cs'!E5</f>
         <v>7.3307000000000002</v>
       </c>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33">
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33">
         <f>'sensi_speed cs'!F5</f>
         <v>9</v>
       </c>
-      <c r="R8" s="33">
+      <c r="S8" s="33">
         <f>'sensi_speed cs'!G5</f>
         <v>12</v>
       </c>
-      <c r="S8" s="33">
+      <c r="T8" s="33">
         <f>'sensi_speed cs'!H5</f>
         <v>8.9352</v>
       </c>
-      <c r="T8" s="34">
+      <c r="U8" s="34">
         <f>'sensi_speed cs'!I5</f>
         <v>0.17957068672217744</v>
       </c>
-      <c r="U8" s="7"/>
       <c r="V8" s="7"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J9" s="45"/>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J9" s="54"/>
       <c r="K9" s="32">
         <f>'sensi_speed cs'!A6</f>
         <v>14</v>
       </c>
       <c r="L9" s="32"/>
-      <c r="M9" s="32">
+      <c r="M9" s="33">
+        <f>'sensi_speed cs'!B6</f>
+        <v>7</v>
+      </c>
+      <c r="N9" s="32">
         <f>'sensi_speed cs'!C6</f>
         <v>16</v>
       </c>
-      <c r="N9" s="32">
+      <c r="O9" s="32">
         <f>'sensi_speed cs'!D6</f>
         <v>1</v>
       </c>
-      <c r="O9" s="32">
+      <c r="P9" s="32">
         <f>'sensi_speed cs'!E6</f>
         <v>7.7404000000000002</v>
       </c>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32">
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32">
         <f>'sensi_speed cs'!F6</f>
         <v>9</v>
       </c>
-      <c r="R9" s="32">
+      <c r="S9" s="32">
         <f>'sensi_speed cs'!G6</f>
         <v>12</v>
       </c>
-      <c r="S9" s="32">
+      <c r="T9" s="32">
         <f>'sensi_speed cs'!H6</f>
         <v>9.3028999999999993</v>
       </c>
-      <c r="T9" s="35">
+      <c r="U9" s="35">
         <f>'sensi_speed cs'!I6</f>
         <v>0.16795837857012322</v>
       </c>
-      <c r="U9" s="7"/>
       <c r="V9" s="7"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J10" s="43" t="s">
+      <c r="W9" s="7"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J10" s="55" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="36">
@@ -1784,156 +1812,172 @@
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="36">
+        <f>'sensi_speed cs'!B12</f>
+        <v>6</v>
+      </c>
+      <c r="N10" s="36">
         <f>'sensi_speed cs'!C12</f>
         <v>18</v>
       </c>
-      <c r="N10" s="36">
+      <c r="O10" s="36">
         <f>'sensi_speed cs'!D12</f>
         <v>1</v>
       </c>
-      <c r="O10" s="36">
+      <c r="P10" s="36">
         <f>'sensi_speed cs'!E12</f>
         <v>6.4054000000000002</v>
       </c>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36">
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36">
         <f>'sensi_speed cs'!F12</f>
         <v>9</v>
       </c>
-      <c r="R10" s="36">
+      <c r="S10" s="36">
         <f>'sensi_speed cs'!G12</f>
         <v>12</v>
       </c>
-      <c r="S10" s="36">
+      <c r="T10" s="36">
         <f>'sensi_speed cs'!H12</f>
         <v>8.0942000000000007</v>
       </c>
-      <c r="T10" s="37">
+      <c r="U10" s="37">
         <f>'sensi_speed cs'!I12</f>
         <v>0.20864322601368887</v>
       </c>
-      <c r="U10" s="7"/>
       <c r="V10" s="7"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J11" s="55"/>
+      <c r="W10" s="7"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J11" s="53"/>
       <c r="K11" s="33">
         <f>'sensi_speed cs'!A14</f>
         <v>20</v>
       </c>
       <c r="L11" s="33"/>
-      <c r="M11" s="33">
+      <c r="M11" s="57">
+        <f>'sensi_speed cs'!B13</f>
+        <v>6</v>
+      </c>
+      <c r="N11" s="33">
         <f>'sensi_speed cs'!C14</f>
         <v>18</v>
       </c>
-      <c r="N11" s="33">
+      <c r="O11" s="33">
         <f>'sensi_speed cs'!D14</f>
         <v>1.3</v>
       </c>
-      <c r="O11" s="33">
+      <c r="P11" s="33">
         <f>'sensi_speed cs'!E14</f>
         <v>6.4127000000000001</v>
       </c>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33">
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33">
         <f>'sensi_speed cs'!F14</f>
         <v>9</v>
       </c>
-      <c r="R11" s="33">
+      <c r="S11" s="33">
         <f>'sensi_speed cs'!G14</f>
         <v>12</v>
       </c>
-      <c r="S11" s="33">
+      <c r="T11" s="33">
         <f>'sensi_speed cs'!H14</f>
         <v>8.5197000000000003</v>
       </c>
-      <c r="T11" s="34">
+      <c r="U11" s="34">
         <f>'sensi_speed cs'!I14</f>
         <v>0.24730917755320025</v>
       </c>
-      <c r="U11" s="7"/>
       <c r="V11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J12" s="55"/>
+      <c r="W11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J12" s="53"/>
       <c r="K12" s="33">
         <f>'sensi_speed cs'!A15</f>
         <v>25</v>
       </c>
       <c r="L12" s="33"/>
-      <c r="M12" s="33">
+      <c r="M12" s="57">
+        <f>'sensi_speed cs'!B14</f>
+        <v>6</v>
+      </c>
+      <c r="N12" s="33">
         <f>'sensi_speed cs'!C15</f>
         <v>18</v>
       </c>
-      <c r="N12" s="33">
+      <c r="O12" s="33">
         <f>'sensi_speed cs'!D15</f>
         <v>0.9</v>
       </c>
-      <c r="O12" s="33">
+      <c r="P12" s="33">
         <f>'sensi_speed cs'!E15</f>
         <v>6.4028999999999998</v>
       </c>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33">
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33">
         <f>'sensi_speed cs'!F15</f>
         <v>9</v>
       </c>
-      <c r="R12" s="33">
+      <c r="S12" s="33">
         <f>'sensi_speed cs'!G15</f>
         <v>12</v>
       </c>
-      <c r="S12" s="33">
+      <c r="T12" s="33">
         <f>'sensi_speed cs'!H15</f>
         <v>8.8023000000000007</v>
       </c>
-      <c r="T12" s="34">
+      <c r="U12" s="34">
         <f>'sensi_speed cs'!I15</f>
         <v>0.27258784635833821</v>
       </c>
-      <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J13" s="55"/>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J13" s="53"/>
       <c r="K13" s="32">
         <f>'sensi_speed cs'!A16</f>
         <v>30</v>
       </c>
       <c r="L13" s="32"/>
-      <c r="M13" s="32">
+      <c r="M13" s="57">
+        <f>'sensi_speed cs'!B15</f>
+        <v>6</v>
+      </c>
+      <c r="N13" s="32">
         <f>'sensi_speed cs'!C16</f>
         <v>18</v>
       </c>
-      <c r="N13" s="32">
+      <c r="O13" s="32">
         <f>'sensi_speed cs'!D16</f>
         <v>1</v>
       </c>
-      <c r="O13" s="32">
+      <c r="P13" s="32">
         <f>'sensi_speed cs'!E16</f>
         <v>6.4105999999999996</v>
       </c>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32">
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32">
         <f>'sensi_speed cs'!F16</f>
         <v>9</v>
       </c>
-      <c r="R13" s="32">
+      <c r="S13" s="32">
         <f>'sensi_speed cs'!G16</f>
         <v>12</v>
       </c>
-      <c r="S13" s="32">
+      <c r="T13" s="32">
         <f>'sensi_speed cs'!H16</f>
         <v>9.0268999999999995</v>
       </c>
-      <c r="T13" s="35">
+      <c r="U13" s="35">
         <f>'sensi_speed cs'!I16</f>
         <v>0.28983371921700696</v>
       </c>
-      <c r="U13" s="7"/>
       <c r="V13" s="7"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J14" s="43" t="s">
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J14" s="55" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="36">
@@ -1942,156 +1986,172 @@
       </c>
       <c r="L14" s="36"/>
       <c r="M14" s="36">
+        <f>'sensi_speed cs'!B23</f>
+        <v>6</v>
+      </c>
+      <c r="N14" s="36">
         <f>'sensi_speed cs'!C23</f>
         <v>18</v>
       </c>
-      <c r="N14" s="36">
+      <c r="O14" s="36">
         <f>'sensi_speed cs'!D23</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O14" s="36">
+      <c r="P14" s="36">
         <f>'sensi_speed cs'!E23</f>
         <v>3.6124999999999998</v>
       </c>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36">
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36">
         <f>'sensi_speed cs'!F23</f>
         <v>9</v>
       </c>
-      <c r="R14" s="36">
+      <c r="S14" s="36">
         <f>'sensi_speed cs'!G23</f>
         <v>11</v>
       </c>
-      <c r="S14" s="36">
+      <c r="T14" s="36">
         <f>'sensi_speed cs'!H23</f>
         <v>5.0346000000000002</v>
       </c>
-      <c r="T14" s="37">
+      <c r="U14" s="37">
         <f>'sensi_speed cs'!I23</f>
         <v>0.28246533984825017</v>
       </c>
-      <c r="U14" s="7"/>
       <c r="V14" s="7"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J15" s="55"/>
+      <c r="W14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J15" s="53"/>
       <c r="K15" s="33">
         <f>'sensi_speed cs'!A24</f>
         <v>150</v>
       </c>
       <c r="L15" s="33"/>
-      <c r="M15" s="33">
+      <c r="M15" s="57">
+        <f>'sensi_speed cs'!B24</f>
+        <v>6</v>
+      </c>
+      <c r="N15" s="33">
         <f>'sensi_speed cs'!C24</f>
         <v>18</v>
       </c>
-      <c r="N15" s="33">
+      <c r="O15" s="33">
         <f>'sensi_speed cs'!D24</f>
         <v>0.8</v>
       </c>
-      <c r="O15" s="33">
+      <c r="P15" s="33">
         <f>'sensi_speed cs'!E24</f>
         <v>5.0114000000000001</v>
       </c>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33">
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33">
         <f>'sensi_speed cs'!F24</f>
         <v>10</v>
       </c>
-      <c r="R15" s="33">
+      <c r="S15" s="33">
         <f>'sensi_speed cs'!G24</f>
         <v>9</v>
       </c>
-      <c r="S15" s="33">
+      <c r="T15" s="33">
         <f>'sensi_speed cs'!H24</f>
         <v>6.7560000000000002</v>
       </c>
-      <c r="T15" s="34">
+      <c r="U15" s="34">
         <f>'sensi_speed cs'!I24</f>
         <v>0.25822972172883363</v>
       </c>
-      <c r="U15" s="7"/>
       <c r="V15" s="7"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="J16" s="55"/>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J16" s="53"/>
       <c r="K16" s="33">
         <f>'sensi_speed cs'!A26</f>
         <v>250</v>
       </c>
       <c r="L16" s="33"/>
-      <c r="M16" s="33">
+      <c r="M16" s="57">
+        <f>'sensi_speed cs'!B25</f>
+        <v>6</v>
+      </c>
+      <c r="N16" s="33">
         <f>'sensi_speed cs'!C26</f>
         <v>18</v>
       </c>
-      <c r="N16" s="33">
+      <c r="O16" s="33">
         <f>'sensi_speed cs'!D26</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O16" s="33">
+      <c r="P16" s="33">
         <f>'sensi_speed cs'!E26</f>
         <v>7.8053999999999997</v>
       </c>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33">
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33">
         <f>'sensi_speed cs'!F26</f>
         <v>9</v>
       </c>
-      <c r="R16" s="33">
+      <c r="S16" s="33">
         <f>'sensi_speed cs'!G26</f>
         <v>12</v>
       </c>
-      <c r="S16" s="33">
+      <c r="T16" s="33">
         <f>'sensi_speed cs'!H26</f>
         <v>10.026400000000001</v>
       </c>
-      <c r="T16" s="34">
+      <c r="U16" s="34">
         <f>'sensi_speed cs'!I26</f>
         <v>0.22151519987233712</v>
       </c>
-      <c r="U16" s="7"/>
       <c r="V16" s="7"/>
-    </row>
-    <row r="17" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J17" s="45"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J17" s="54"/>
       <c r="K17" s="32">
         <f>'sensi_speed cs'!A27</f>
         <v>300</v>
       </c>
       <c r="L17" s="32"/>
-      <c r="M17" s="32">
+      <c r="M17" s="57">
+        <f>'sensi_speed cs'!B26</f>
+        <v>6</v>
+      </c>
+      <c r="N17" s="32">
         <f>'sensi_speed cs'!C27</f>
         <v>19</v>
       </c>
-      <c r="N17" s="32">
+      <c r="O17" s="32">
         <f>'sensi_speed cs'!D27</f>
         <v>1.4</v>
       </c>
-      <c r="O17" s="32">
+      <c r="P17" s="32">
         <f>'sensi_speed cs'!E27</f>
         <v>9.1647999999999996</v>
       </c>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32">
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32">
         <f>'sensi_speed cs'!F27</f>
         <v>9</v>
       </c>
-      <c r="R17" s="32">
+      <c r="S17" s="32">
         <f>'sensi_speed cs'!G27</f>
         <v>13</v>
       </c>
-      <c r="S17" s="32">
+      <c r="T17" s="32">
         <f>'sensi_speed cs'!H27</f>
         <v>11.72</v>
       </c>
-      <c r="T17" s="35">
+      <c r="U17" s="35">
         <f>'sensi_speed cs'!I27</f>
         <v>0.21802047781569975</v>
       </c>
-      <c r="U17" s="7"/>
       <c r="V17" s="7"/>
-    </row>
-    <row r="18" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J18" s="43" t="s">
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J18" s="55" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="36">
@@ -2100,156 +2160,172 @@
       </c>
       <c r="L18" s="36"/>
       <c r="M18" s="36">
+        <f>'sensi_speed cs'!B35</f>
+        <v>6</v>
+      </c>
+      <c r="N18" s="36">
         <f>'sensi_speed cs'!C34</f>
         <v>18</v>
       </c>
-      <c r="N18" s="36">
+      <c r="O18" s="36">
         <f>'sensi_speed cs'!D34</f>
         <v>0.9</v>
       </c>
-      <c r="O18" s="36">
+      <c r="P18" s="36">
         <f>'sensi_speed cs'!E34</f>
         <v>6.4108999999999998</v>
       </c>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36">
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36">
         <f>'sensi_speed cs'!F34</f>
         <v>9</v>
       </c>
-      <c r="R18" s="36">
+      <c r="S18" s="36">
         <f>'sensi_speed cs'!G34</f>
         <v>13</v>
       </c>
-      <c r="S18" s="36">
+      <c r="T18" s="36">
         <f>'sensi_speed cs'!H34</f>
         <v>8.2538</v>
       </c>
-      <c r="T18" s="37">
+      <c r="U18" s="37">
         <f>'sensi_speed cs'!I34</f>
         <v>0.22327897453294243</v>
       </c>
-      <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-    </row>
-    <row r="19" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J19" s="55"/>
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J19" s="53"/>
       <c r="K19" s="33">
         <f>'sensi_speed cs'!A36</f>
         <v>2500</v>
       </c>
       <c r="L19" s="33"/>
-      <c r="M19" s="33">
+      <c r="M19" s="57">
+        <f>'sensi_speed cs'!B36</f>
+        <v>6</v>
+      </c>
+      <c r="N19" s="33">
         <f>'sensi_speed cs'!C36</f>
         <v>18</v>
       </c>
-      <c r="N19" s="33">
+      <c r="O19" s="33">
         <f>'sensi_speed cs'!D36</f>
         <v>0.9</v>
       </c>
-      <c r="O19" s="33">
+      <c r="P19" s="33">
         <f>'sensi_speed cs'!E36</f>
         <v>6.4051999999999998</v>
       </c>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33">
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33">
         <f>'sensi_speed cs'!F36</f>
         <v>9</v>
       </c>
-      <c r="R19" s="33">
+      <c r="S19" s="33">
         <f>'sensi_speed cs'!G36</f>
         <v>12</v>
       </c>
-      <c r="S19" s="33">
+      <c r="T19" s="33">
         <f>'sensi_speed cs'!H36</f>
         <v>8.3809000000000005</v>
       </c>
-      <c r="T19" s="34">
+      <c r="U19" s="34">
         <f>'sensi_speed cs'!I36</f>
         <v>0.23573840518321429</v>
       </c>
-      <c r="U19" s="7"/>
       <c r="V19" s="7"/>
-    </row>
-    <row r="20" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J20" s="55"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J20" s="53"/>
       <c r="K20" s="33">
         <f>'sensi_speed cs'!A37</f>
         <v>3000</v>
       </c>
       <c r="L20" s="33"/>
-      <c r="M20" s="33">
+      <c r="M20" s="57">
+        <f>'sensi_speed cs'!B37</f>
+        <v>6</v>
+      </c>
+      <c r="N20" s="33">
         <f>'sensi_speed cs'!C37</f>
         <v>18</v>
       </c>
-      <c r="N20" s="33">
+      <c r="O20" s="33">
         <f>'sensi_speed cs'!D37</f>
         <v>1.4</v>
       </c>
-      <c r="O20" s="33">
+      <c r="P20" s="33">
         <f>'sensi_speed cs'!E37</f>
         <v>6.4229000000000003</v>
       </c>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33">
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33">
         <f>'sensi_speed cs'!F37</f>
         <v>9</v>
       </c>
-      <c r="R20" s="33">
+      <c r="S20" s="33">
         <f>'sensi_speed cs'!G37</f>
         <v>12</v>
       </c>
-      <c r="S20" s="33">
+      <c r="T20" s="33">
         <f>'sensi_speed cs'!H37</f>
         <v>8.4442000000000004</v>
       </c>
-      <c r="T20" s="34">
+      <c r="U20" s="34">
         <f>'sensi_speed cs'!I37</f>
         <v>0.23937140285639846</v>
       </c>
-      <c r="U20" s="7"/>
       <c r="V20" s="7"/>
-    </row>
-    <row r="21" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J21" s="55"/>
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J21" s="53"/>
       <c r="K21" s="32">
         <f>'sensi_speed cs'!A38</f>
         <v>3500</v>
       </c>
       <c r="L21" s="32"/>
       <c r="M21" s="32">
+        <f>'sensi_speed cs'!B38</f>
+        <v>6</v>
+      </c>
+      <c r="N21" s="32">
         <f>'sensi_speed cs'!C38</f>
         <v>18</v>
       </c>
-      <c r="N21" s="32">
+      <c r="O21" s="32">
         <f>'sensi_speed cs'!D38</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O21" s="32">
+      <c r="P21" s="32">
         <f>'sensi_speed cs'!E38</f>
         <v>6.4227999999999996</v>
       </c>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32">
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32">
         <f>'sensi_speed cs'!F38</f>
         <v>9</v>
       </c>
-      <c r="R21" s="32">
+      <c r="S21" s="32">
         <f>'sensi_speed cs'!G38</f>
         <v>11</v>
       </c>
-      <c r="S21" s="32">
+      <c r="T21" s="32">
         <f>'sensi_speed cs'!H38</f>
         <v>8.4097000000000008</v>
       </c>
-      <c r="T21" s="35">
+      <c r="U21" s="35">
         <f>'sensi_speed cs'!I38</f>
         <v>0.23626288690440814</v>
       </c>
-      <c r="U21" s="7"/>
       <c r="V21" s="7"/>
-    </row>
-    <row r="22" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J22" s="43" t="str">
+      <c r="W21" s="7"/>
+    </row>
+    <row r="22" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J22" s="55" t="str">
         <f>'sensi_speed cs'!A42</f>
         <v>cs</v>
       </c>
@@ -2258,157 +2334,173 @@
         <v>20</v>
       </c>
       <c r="L22" s="36"/>
-      <c r="M22" s="36">
+      <c r="M22" s="57">
+        <f>'sensi_speed cs'!B44</f>
+        <v>6</v>
+      </c>
+      <c r="N22" s="36">
         <f>'sensi_speed cs'!C43</f>
         <v>18</v>
       </c>
-      <c r="N22" s="36">
+      <c r="O22" s="36">
         <f>'sensi_speed cs'!D43</f>
         <v>0.9</v>
       </c>
-      <c r="O22" s="36">
+      <c r="P22" s="36">
         <f>'sensi_speed cs'!E43</f>
         <v>6.4108999999999998</v>
       </c>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36">
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36">
         <f>'sensi_speed cs'!F43</f>
         <v>9</v>
       </c>
-      <c r="R22" s="36">
+      <c r="S22" s="36">
         <f>'sensi_speed cs'!G43</f>
         <v>13</v>
       </c>
-      <c r="S22" s="36">
+      <c r="T22" s="36">
         <f>'sensi_speed cs'!H43</f>
         <v>8.3396000000000008</v>
       </c>
-      <c r="T22" s="37">
+      <c r="U22" s="37">
         <f>'sensi_speed cs'!I43</f>
         <v>0.23127008489615819</v>
       </c>
-      <c r="U22" s="7"/>
       <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J23" s="55"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J23" s="53"/>
       <c r="K23" s="33">
         <f>'sensi_speed cs'!A44</f>
         <v>30</v>
       </c>
       <c r="L23" s="33"/>
-      <c r="M23" s="33">
+      <c r="M23" s="57">
+        <f>'sensi_speed cs'!B45</f>
+        <v>6</v>
+      </c>
+      <c r="N23" s="33">
         <f>'sensi_speed cs'!C44</f>
         <v>18</v>
       </c>
-      <c r="N23" s="33">
+      <c r="O23" s="33">
         <f>'sensi_speed cs'!D44</f>
         <v>1</v>
       </c>
-      <c r="O23" s="33">
+      <c r="P23" s="33">
         <f>'sensi_speed cs'!E44</f>
         <v>6.4054000000000002</v>
       </c>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33">
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33">
         <f>'sensi_speed cs'!F44</f>
         <v>9</v>
       </c>
-      <c r="R23" s="33">
+      <c r="S23" s="33">
         <f>'sensi_speed cs'!G44</f>
         <v>12</v>
       </c>
-      <c r="S23" s="33">
+      <c r="T23" s="33">
         <f>'sensi_speed cs'!H44</f>
         <v>8.3114000000000008</v>
       </c>
-      <c r="T23" s="34">
+      <c r="U23" s="34">
         <f>'sensi_speed cs'!I44</f>
         <v>0.22932357966166955</v>
       </c>
-      <c r="U23" s="7"/>
       <c r="V23" s="7"/>
-    </row>
-    <row r="24" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J24" s="55"/>
+      <c r="W23" s="7"/>
+    </row>
+    <row r="24" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J24" s="53"/>
       <c r="K24" s="33">
         <f>'sensi_speed cs'!A46</f>
         <v>50</v>
       </c>
       <c r="L24" s="33"/>
-      <c r="M24" s="33">
+      <c r="M24" s="57">
+        <f>'sensi_speed cs'!B46</f>
+        <v>6</v>
+      </c>
+      <c r="N24" s="33">
         <f>'sensi_speed cs'!C46</f>
         <v>18</v>
       </c>
-      <c r="N24" s="33">
+      <c r="O24" s="33">
         <f>'sensi_speed cs'!D46</f>
         <v>1.4</v>
       </c>
-      <c r="O24" s="33">
+      <c r="P24" s="33">
         <f>'sensi_speed cs'!E46</f>
         <v>6.4229000000000003</v>
       </c>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33">
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33">
         <f>'sensi_speed cs'!F46</f>
         <v>9</v>
       </c>
-      <c r="R24" s="33">
+      <c r="S24" s="33">
         <f>'sensi_speed cs'!G46</f>
         <v>12</v>
       </c>
-      <c r="S24" s="33">
+      <c r="T24" s="33">
         <f>'sensi_speed cs'!H46</f>
         <v>8.3124000000000002</v>
       </c>
-      <c r="T24" s="34">
+      <c r="U24" s="34">
         <f>'sensi_speed cs'!I46</f>
         <v>0.22731100524517586</v>
       </c>
-      <c r="U24" s="7"/>
       <c r="V24" s="7"/>
-    </row>
-    <row r="25" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J25" s="45"/>
+      <c r="W24" s="7"/>
+    </row>
+    <row r="25" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J25" s="54"/>
       <c r="K25" s="32">
         <f>'sensi_speed cs'!A47</f>
         <v>60</v>
       </c>
       <c r="L25" s="32"/>
       <c r="M25" s="32">
+        <f>'sensi_speed cs'!B47</f>
+        <v>6</v>
+      </c>
+      <c r="N25" s="32">
         <f>'sensi_speed cs'!C47</f>
         <v>18</v>
       </c>
-      <c r="N25" s="32">
+      <c r="O25" s="32">
         <f>'sensi_speed cs'!D47</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O25" s="32">
+      <c r="P25" s="32">
         <f>'sensi_speed cs'!E47</f>
         <v>6.4227999999999996</v>
       </c>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32">
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32">
         <f>'sensi_speed cs'!F47</f>
         <v>9</v>
       </c>
-      <c r="R25" s="32">
+      <c r="S25" s="32">
         <f>'sensi_speed cs'!G47</f>
         <v>12</v>
       </c>
-      <c r="S25" s="32">
+      <c r="T25" s="32">
         <f>'sensi_speed cs'!H47</f>
         <v>8.2928999999999995</v>
       </c>
-      <c r="T25" s="35">
+      <c r="U25" s="35">
         <f>'sensi_speed cs'!I47</f>
         <v>0.22550615586827286</v>
       </c>
-      <c r="U25" s="7"/>
       <c r="V25" s="7"/>
-    </row>
-    <row r="26" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J26" s="44" t="s">
+      <c r="W25" s="7"/>
+    </row>
+    <row r="26" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J26" s="53" t="s">
         <v>50</v>
       </c>
       <c r="K26" s="36">
@@ -2417,159 +2509,175 @@
       </c>
       <c r="L26" s="36"/>
       <c r="M26" s="36">
+        <f>'sensi_speed cs'!B52</f>
+        <v>8</v>
+      </c>
+      <c r="N26" s="36">
         <f>'sensi_speed cs'!C52</f>
         <v>12</v>
       </c>
-      <c r="N26" s="36">
+      <c r="O26" s="36">
         <f>'sensi_speed cs'!D52</f>
         <v>0.6</v>
       </c>
-      <c r="O26" s="36">
+      <c r="P26" s="36">
         <f>'sensi_speed cs'!E52</f>
         <v>5.9827000000000004</v>
       </c>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36">
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36">
         <f>'sensi_speed cs'!F52</f>
         <v>10</v>
       </c>
-      <c r="R26" s="36">
+      <c r="S26" s="36">
         <f>'sensi_speed cs'!G52</f>
         <v>8</v>
       </c>
-      <c r="S26" s="36">
+      <c r="T26" s="36">
         <f>'sensi_speed cs'!H52</f>
         <v>7.4097</v>
       </c>
-      <c r="T26" s="37">
+      <c r="U26" s="37">
         <f>'sensi_speed cs'!I52</f>
         <v>0.19258539482030307</v>
       </c>
-      <c r="U26" s="7"/>
       <c r="V26" s="7"/>
-    </row>
-    <row r="27" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J27" s="44"/>
+      <c r="W26" s="7"/>
+    </row>
+    <row r="27" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J27" s="53"/>
       <c r="K27" s="33">
         <f>'sensi_speed cs'!A54</f>
         <v>0.6</v>
       </c>
       <c r="L27" s="33"/>
-      <c r="M27" s="33">
+      <c r="M27" s="57">
+        <f>'sensi_speed cs'!B54</f>
+        <v>5</v>
+      </c>
+      <c r="N27" s="33">
         <f>'sensi_speed cs'!C54</f>
         <v>21</v>
       </c>
-      <c r="N27" s="33">
+      <c r="O27" s="33">
         <f>'sensi_speed cs'!D54</f>
         <v>1.3</v>
       </c>
-      <c r="O27" s="33">
+      <c r="P27" s="33">
         <f>'sensi_speed cs'!E54</f>
         <v>7.0849000000000002</v>
       </c>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33">
+      <c r="Q27" s="33"/>
+      <c r="R27" s="33">
         <f>'sensi_speed cs'!F54</f>
         <v>9</v>
       </c>
-      <c r="R27" s="33">
+      <c r="S27" s="33">
         <f>'sensi_speed cs'!G54</f>
         <v>13</v>
       </c>
-      <c r="S27" s="33">
+      <c r="T27" s="33">
         <f>'sensi_speed cs'!H54</f>
         <v>9.1378000000000004</v>
       </c>
-      <c r="T27" s="34">
+      <c r="U27" s="34">
         <f>'sensi_speed cs'!I54</f>
         <v>0.2246602026746044</v>
       </c>
-      <c r="U27" s="7"/>
       <c r="V27" s="7"/>
-    </row>
-    <row r="28" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J28" s="44"/>
+      <c r="W27" s="7"/>
+    </row>
+    <row r="28" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J28" s="53"/>
       <c r="K28" s="33">
         <f>'sensi_speed cs'!A55</f>
         <v>0.8</v>
       </c>
       <c r="L28" s="33"/>
-      <c r="M28" s="33">
+      <c r="M28" s="57">
+        <f>'sensi_speed cs'!B55</f>
+        <v>6</v>
+      </c>
+      <c r="N28" s="33">
         <f>'sensi_speed cs'!C55</f>
         <v>24</v>
       </c>
-      <c r="N28" s="33">
+      <c r="O28" s="33">
         <f>'sensi_speed cs'!D55</f>
         <v>1.4</v>
       </c>
-      <c r="O28" s="33">
+      <c r="P28" s="33">
         <f>'sensi_speed cs'!E55</f>
         <v>7.3578000000000001</v>
       </c>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33">
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33">
         <f>'sensi_speed cs'!F55</f>
         <v>8</v>
       </c>
-      <c r="R28" s="33">
+      <c r="S28" s="33">
         <f>'sensi_speed cs'!G55</f>
         <v>15</v>
       </c>
-      <c r="S28" s="33">
+      <c r="T28" s="33">
         <f>'sensi_speed cs'!H55</f>
         <v>10.007199999999999</v>
       </c>
-      <c r="T28" s="34">
+      <c r="U28" s="34">
         <f>'sensi_speed cs'!I55</f>
         <v>0.26474938044607876</v>
       </c>
-      <c r="U28" s="7"/>
-      <c r="V28" s="58" t="str">
+      <c r="V28" s="7"/>
+      <c r="W28" s="46" t="str">
         <f>'sensi_speed cs'!K54</f>
         <v>退化速度越大，越需要细致的观测interval来进行时刻检测。而Model B的检测成本较高，没办法实行细致检测，导致cost rate越大。</v>
       </c>
     </row>
-    <row r="29" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J29" s="45"/>
+    <row r="29" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J29" s="54"/>
       <c r="K29" s="32">
         <f>'sensi_speed cs'!A56</f>
         <v>1</v>
       </c>
       <c r="L29" s="32"/>
       <c r="M29" s="32">
+        <f>'sensi_speed cs'!B56</f>
+        <v>4</v>
+      </c>
+      <c r="N29" s="32">
         <f>'sensi_speed cs'!C56</f>
         <v>29</v>
       </c>
-      <c r="N29" s="32">
+      <c r="O29" s="32">
         <f>'sensi_speed cs'!D56</f>
         <v>2.6</v>
       </c>
-      <c r="O29" s="32">
+      <c r="P29" s="32">
         <f>'sensi_speed cs'!E56</f>
         <v>7.9672999999999998</v>
       </c>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32">
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32">
         <f>'sensi_speed cs'!F56</f>
         <v>10</v>
       </c>
-      <c r="R29" s="32">
+      <c r="S29" s="32">
         <f>'sensi_speed cs'!G56</f>
         <v>12</v>
       </c>
-      <c r="S29" s="32">
+      <c r="T29" s="32">
         <f>'sensi_speed cs'!H56</f>
         <v>10.875299999999999</v>
       </c>
-      <c r="T29" s="35">
+      <c r="U29" s="35">
         <f>'sensi_speed cs'!I56</f>
         <v>0.26739492243892121</v>
       </c>
-      <c r="U29" s="7"/>
       <c r="V29" s="7"/>
-    </row>
-    <row r="30" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J30" s="43" t="s">
+      <c r="W29" s="7"/>
+    </row>
+    <row r="30" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J30" s="55" t="s">
         <v>51</v>
       </c>
       <c r="K30" s="36">
@@ -2578,159 +2686,175 @@
       </c>
       <c r="L30" s="36"/>
       <c r="M30" s="36">
+        <f>'sensi_speed cs'!B62</f>
+        <v>7</v>
+      </c>
+      <c r="N30" s="36">
         <f>'sensi_speed cs'!C62</f>
         <v>20</v>
       </c>
-      <c r="N30" s="36">
+      <c r="O30" s="36">
         <f>'sensi_speed cs'!D62</f>
         <v>1</v>
       </c>
-      <c r="O30" s="36">
+      <c r="P30" s="36">
         <f>'sensi_speed cs'!E62</f>
         <v>5.9623999999999997</v>
       </c>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36">
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36">
         <f>'sensi_speed cs'!F62</f>
         <v>11</v>
       </c>
-      <c r="R30" s="36">
+      <c r="S30" s="36">
         <f>'sensi_speed cs'!G62</f>
         <v>13</v>
       </c>
-      <c r="S30" s="36">
+      <c r="T30" s="36">
         <f>'sensi_speed cs'!H62</f>
         <v>7.2706999999999997</v>
       </c>
-      <c r="T30" s="37">
+      <c r="U30" s="37">
         <f>'sensi_speed cs'!I62</f>
         <v>0.17994140866766611</v>
       </c>
-      <c r="U30" s="7"/>
       <c r="V30" s="7"/>
-    </row>
-    <row r="31" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J31" s="55"/>
+      <c r="W30" s="7"/>
+    </row>
+    <row r="31" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J31" s="53"/>
       <c r="K31" s="33">
         <f>'sensi_speed cs'!A63</f>
         <v>2.4</v>
       </c>
       <c r="L31" s="33"/>
       <c r="M31" s="33">
+        <f>'sensi_speed cs'!B63</f>
+        <v>6</v>
+      </c>
+      <c r="N31" s="33">
         <f>'sensi_speed cs'!C63</f>
         <v>20</v>
       </c>
-      <c r="N31" s="33">
+      <c r="O31" s="33">
         <f>'sensi_speed cs'!D63</f>
         <v>1</v>
       </c>
-      <c r="O31" s="33">
+      <c r="P31" s="33">
         <f>'sensi_speed cs'!E63</f>
         <v>6.2030000000000003</v>
       </c>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33">
+      <c r="Q31" s="33"/>
+      <c r="R31" s="33">
         <f>'sensi_speed cs'!F63</f>
         <v>10</v>
       </c>
-      <c r="R31" s="33">
+      <c r="S31" s="33">
         <f>'sensi_speed cs'!G63</f>
         <v>12</v>
       </c>
-      <c r="S31" s="33">
+      <c r="T31" s="33">
         <f>'sensi_speed cs'!H63</f>
         <v>7.8150000000000004</v>
       </c>
-      <c r="T31" s="34">
+      <c r="U31" s="34">
         <f>'sensi_speed cs'!I63</f>
         <v>0.20626999360204734</v>
       </c>
-      <c r="U31" s="7"/>
       <c r="V31" s="7"/>
-    </row>
-    <row r="32" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J32" s="55"/>
+      <c r="W31" s="7"/>
+    </row>
+    <row r="32" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J32" s="53"/>
       <c r="K32" s="33">
         <f>'sensi_speed cs'!A65</f>
         <v>3</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="33">
+        <f>'sensi_speed cs'!B65</f>
+        <v>5</v>
+      </c>
+      <c r="N32" s="33">
         <f>'sensi_speed cs'!C65</f>
         <v>19</v>
       </c>
-      <c r="N32" s="33">
+      <c r="O32" s="33">
         <f>'sensi_speed cs'!D65</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O32" s="33">
+      <c r="P32" s="33">
         <f>'sensi_speed cs'!E65</f>
         <v>6.6249000000000002</v>
       </c>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="33">
+      <c r="Q32" s="33"/>
+      <c r="R32" s="33">
         <f>'sensi_speed cs'!F65</f>
         <v>8</v>
       </c>
-      <c r="R32" s="33">
+      <c r="S32" s="33">
         <f>'sensi_speed cs'!G65</f>
         <v>12</v>
       </c>
-      <c r="S32" s="33">
+      <c r="T32" s="33">
         <f>'sensi_speed cs'!H65</f>
         <v>8.8216000000000001</v>
       </c>
-      <c r="T32" s="34">
+      <c r="U32" s="34">
         <f>'sensi_speed cs'!I65</f>
         <v>0.24901378434751065</v>
       </c>
-      <c r="U32" s="7"/>
-      <c r="V32" s="58" t="str">
+      <c r="V32" s="7"/>
+      <c r="W32" s="46" t="str">
         <f>'sensi_speed cs'!K64</f>
         <v>同样是检测成本过高的问题</v>
       </c>
     </row>
-    <row r="33" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J33" s="45"/>
+    <row r="33" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J33" s="54"/>
       <c r="K33" s="32">
         <f>'sensi_speed cs'!A66</f>
         <v>3.3</v>
       </c>
       <c r="L33" s="32"/>
       <c r="M33" s="32">
+        <f>'sensi_speed cs'!B66</f>
+        <v>5</v>
+      </c>
+      <c r="N33" s="32">
         <f>'sensi_speed cs'!C66</f>
         <v>18</v>
       </c>
-      <c r="N33" s="32">
+      <c r="O33" s="32">
         <f>'sensi_speed cs'!D66</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O33" s="32">
+      <c r="P33" s="32">
         <f>'sensi_speed cs'!E66</f>
         <v>6.7849000000000004</v>
       </c>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32">
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32">
         <f>'sensi_speed cs'!F66</f>
         <v>7</v>
       </c>
-      <c r="R33" s="32">
+      <c r="S33" s="32">
         <f>'sensi_speed cs'!G66</f>
         <v>13</v>
       </c>
-      <c r="S33" s="32">
+      <c r="T33" s="32">
         <f>'sensi_speed cs'!H66</f>
         <v>9.3912999999999993</v>
       </c>
-      <c r="T33" s="35">
+      <c r="U33" s="35">
         <f>'sensi_speed cs'!I66</f>
         <v>0.27753346182104704</v>
       </c>
-      <c r="U33" s="7"/>
       <c r="V33" s="7"/>
-    </row>
-    <row r="34" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J34" s="45" t="s">
+      <c r="W33" s="7"/>
+    </row>
+    <row r="34" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J34" s="54" t="s">
         <v>52</v>
       </c>
       <c r="K34" s="36">
@@ -2739,208 +2863,222 @@
       </c>
       <c r="L34" s="36"/>
       <c r="M34" s="36">
+        <f>'sensi_speed cs'!B71</f>
+        <v>7</v>
+      </c>
+      <c r="N34" s="36">
         <f>'sensi_speed cs'!C71</f>
         <v>15</v>
       </c>
-      <c r="N34" s="36">
+      <c r="O34" s="36">
         <f>'sensi_speed cs'!D71</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O34" s="36">
+      <c r="P34" s="36">
         <f>'sensi_speed cs'!E71</f>
         <v>7.5206</v>
       </c>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36">
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36">
         <f>'sensi_speed cs'!F71</f>
         <v>9</v>
       </c>
-      <c r="R34" s="36">
+      <c r="S34" s="36">
         <f>'sensi_speed cs'!G71</f>
         <v>11</v>
       </c>
-      <c r="S34" s="36">
+      <c r="T34" s="36">
         <f>'sensi_speed cs'!H71</f>
         <v>8.9542999999999999</v>
       </c>
-      <c r="T34" s="37">
+      <c r="U34" s="37">
         <f>'sensi_speed cs'!I71</f>
         <v>0.16011301832639066</v>
       </c>
-      <c r="U34" s="7"/>
       <c r="V34" s="7"/>
-    </row>
-    <row r="35" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J35" s="45"/>
+      <c r="W34" s="7"/>
+    </row>
+    <row r="35" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J35" s="54"/>
       <c r="K35" s="33">
         <f>'sensi_speed cs'!A72</f>
         <v>30</v>
       </c>
       <c r="L35" s="33"/>
       <c r="M35" s="33">
+        <f>'sensi_speed cs'!B72</f>
+        <v>6</v>
+      </c>
+      <c r="N35" s="33">
         <f>'sensi_speed cs'!C72</f>
         <v>18</v>
       </c>
-      <c r="N35" s="33">
+      <c r="O35" s="33">
         <f>'sensi_speed cs'!D72</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O35" s="33">
+      <c r="P35" s="33">
         <f>'sensi_speed cs'!E72</f>
         <v>6.8738999999999999</v>
       </c>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33">
+      <c r="Q35" s="33"/>
+      <c r="R35" s="33">
         <f>'sensi_speed cs'!F72</f>
         <v>9</v>
       </c>
-      <c r="R35" s="33">
+      <c r="S35" s="33">
         <f>'sensi_speed cs'!G72</f>
         <v>11</v>
       </c>
-      <c r="S35" s="33">
+      <c r="T35" s="33">
         <f>'sensi_speed cs'!H72</f>
         <v>8.6221999999999994</v>
       </c>
-      <c r="T35" s="34">
+      <c r="U35" s="34">
         <f>'sensi_speed cs'!I72</f>
         <v>0.20276727517338958</v>
       </c>
-      <c r="U35" s="7"/>
-      <c r="V35" s="58" t="str">
+      <c r="V35" s="7"/>
+      <c r="W35" s="46" t="str">
         <f>'sensi_speed cs'!K72</f>
         <v>检测成本，defect时间越靠后，MI无效开销越多</v>
       </c>
     </row>
-    <row r="36" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J36" s="45"/>
+    <row r="36" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J36" s="54"/>
       <c r="K36" s="33">
         <f>'sensi_speed cs'!A74</f>
         <v>38</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="33">
+        <f>'sensi_speed cs'!B74</f>
+        <v>6</v>
+      </c>
+      <c r="N36" s="33">
         <f>'sensi_speed cs'!C74</f>
         <v>18</v>
       </c>
-      <c r="N36" s="33">
+      <c r="O36" s="33">
         <f>'sensi_speed cs'!D74</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O36" s="33">
+      <c r="P36" s="33">
         <f>'sensi_speed cs'!E74</f>
         <v>6.0797999999999996</v>
       </c>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33">
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33">
         <f>'sensi_speed cs'!F74</f>
         <v>9</v>
       </c>
-      <c r="R36" s="33">
+      <c r="S36" s="33">
         <f>'sensi_speed cs'!G74</f>
         <v>13</v>
       </c>
-      <c r="S36" s="33">
+      <c r="T36" s="33">
         <f>'sensi_speed cs'!H74</f>
         <v>8.1298999999999992</v>
       </c>
-      <c r="T36" s="34">
+      <c r="U36" s="34">
         <f>'sensi_speed cs'!I74</f>
         <v>0.25216792334469057</v>
       </c>
-      <c r="U36" s="7"/>
       <c r="V36" s="7"/>
-    </row>
-    <row r="37" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J37" s="45"/>
+      <c r="W36" s="7"/>
+    </row>
+    <row r="37" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J37" s="54"/>
       <c r="K37" s="32">
         <f>'sensi_speed cs'!A75</f>
         <v>42</v>
       </c>
       <c r="L37" s="32"/>
       <c r="M37" s="32">
+        <f>'sensi_speed cs'!B75</f>
+        <v>6</v>
+      </c>
+      <c r="N37" s="32">
         <f>'sensi_speed cs'!C75</f>
         <v>18</v>
       </c>
-      <c r="N37" s="32">
+      <c r="O37" s="32">
         <f>'sensi_speed cs'!D75</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O37" s="32">
+      <c r="P37" s="32">
         <f>'sensi_speed cs'!E75</f>
         <v>5.8022</v>
       </c>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32">
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32">
         <f>'sensi_speed cs'!F75</f>
         <v>9</v>
       </c>
-      <c r="R37" s="32">
+      <c r="S37" s="32">
         <f>'sensi_speed cs'!G75</f>
         <v>13</v>
       </c>
-      <c r="S37" s="32">
+      <c r="T37" s="32">
         <f>'sensi_speed cs'!H75</f>
         <v>7.9333999999999998</v>
       </c>
-      <c r="T37" s="35">
+      <c r="U37" s="35">
         <f>'sensi_speed cs'!I75</f>
         <v>0.26863639801346206</v>
       </c>
-      <c r="U37" s="7"/>
       <c r="V37" s="7"/>
-    </row>
-    <row r="38" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J38" s="54"/>
-      <c r="U38" s="7"/>
+      <c r="W37" s="7"/>
+    </row>
+    <row r="38" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J38" s="45"/>
       <c r="V38" s="7"/>
-    </row>
-    <row r="39" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J39" s="56"/>
-      <c r="U39" s="7"/>
-    </row>
-    <row r="40" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J40" s="56"/>
-      <c r="U40" s="7"/>
-    </row>
-    <row r="41" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J41" s="56"/>
-      <c r="U41" s="7"/>
-    </row>
-    <row r="42" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J42" s="56"/>
-      <c r="U42" s="7"/>
-    </row>
-    <row r="43" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J43" s="56"/>
-      <c r="U43" s="7"/>
-    </row>
-    <row r="44" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J44" s="56"/>
-      <c r="U44" s="7"/>
-    </row>
-    <row r="45" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J45" s="57"/>
+      <c r="W38" s="7"/>
+    </row>
+    <row r="39" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J39" s="45"/>
+      <c r="V39" s="7"/>
+    </row>
+    <row r="40" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J40" s="45"/>
+      <c r="V40" s="7"/>
+    </row>
+    <row r="41" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J41" s="45"/>
+      <c r="V41" s="7"/>
+    </row>
+    <row r="42" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J42" s="45"/>
+      <c r="V42" s="7"/>
+    </row>
+    <row r="43" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J43" s="45"/>
+      <c r="V43" s="7"/>
+    </row>
+    <row r="44" spans="10:23" x14ac:dyDescent="0.3">
+      <c r="J44" s="45"/>
+      <c r="V44" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J22:J25"/>
+    <mergeCell ref="J30:J33"/>
+    <mergeCell ref="J26:J29"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="J5:J9"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J3:K4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="J5:J9"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="J22:J25"/>
-    <mergeCell ref="J30:J33"/>
-    <mergeCell ref="J26:J29"/>
-    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="L3:P3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2948,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27BF723-D6DC-4608-ABE2-E81C591742E9}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>